<commit_message>
added msgbox with complete
</commit_message>
<xml_diff>
--- a/11_20_2020 BRWD FJ RAW.xlsx
+++ b/11_20_2020 BRWD FJ RAW.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,65 +461,80 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>ClerkFileNumber</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Plaintiff</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Amount $</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Case #</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Def First</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Def MI</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Def Last</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Mailing Address</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>City</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>ST</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Zip</t>
         </is>
@@ -542,46 +557,55 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
         <v>116877265</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="J2" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
         <is>
           <t>COWE-08-020657</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>Adrianna</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>Jeffery</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -600,58 +624,67 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
         <v>116877266</v>
       </c>
-      <c r="G3" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H3" t="inlineStr">
+      <c r="J3" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>Asset Acceptance LLC</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>COWE-06-001326</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>Lauren</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Burley</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>2354 N. Military Trail #210</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>West Palm Beach</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R3" t="n">
+      <c r="U3" t="n">
         <v>33409</v>
       </c>
     </row>
@@ -672,58 +705,67 @@
         <v>2</v>
       </c>
       <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="n">
         <v>116877268</v>
       </c>
-      <c r="G4" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H4" t="inlineStr">
+      <c r="J4" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>Lien Source LLC</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>COSO-20-010813</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>Jean</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr">
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>Elie</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>230 NE 61 Street</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>Ft Lauderdale</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>33334-1929</t>
         </is>
@@ -746,58 +788,67 @@
         <v>3</v>
       </c>
       <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" t="n">
         <v>116877273</v>
       </c>
-      <c r="G5" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H5" t="inlineStr">
+      <c r="J5" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>COSO-19-007468</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>Humberto</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>Mesa</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>2216 Taft Street</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>Hollywood</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>33020-2641</t>
         </is>
@@ -820,46 +871,55 @@
         <v>4</v>
       </c>
       <c r="F6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" t="n">
         <v>116877290</v>
       </c>
-      <c r="G6" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H6" t="inlineStr">
+      <c r="J6" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>Progressive Select Insurance Company</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
         <is>
           <t>COWE-15-005648</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>Doreen</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>Annmarie</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>Goodgame</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -878,42 +938,51 @@
         <v>5</v>
       </c>
       <c r="F7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>5</v>
+      </c>
+      <c r="I7" t="n">
         <v>116877295</v>
       </c>
-      <c r="G7" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H7" t="inlineStr">
+      <c r="J7" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>Lago Funding Corp</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>COSO-17-004512</t>
-        </is>
-      </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Valerie</t>
+          <t>FJ</t>
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
+          <t>COSO-17-004512</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Valerie</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
+        <is>
           <t>Vieux</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -932,58 +1001,67 @@
         <v>6</v>
       </c>
       <c r="F8" t="n">
+        <v>6</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6</v>
+      </c>
+      <c r="I8" t="n">
         <v>116877319</v>
       </c>
-      <c r="G8" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H8" t="inlineStr">
+      <c r="J8" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>COSO-19-003421</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>Calin</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr">
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr">
         <is>
           <t>Romosan</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="R8" t="inlineStr">
         <is>
           <t>608 S CRESCENT DRIVE</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R8" t="n">
+      <c r="U8" t="n">
         <v>33021</v>
       </c>
     </row>
@@ -1004,62 +1082,71 @@
         <v>7</v>
       </c>
       <c r="F9" t="n">
+        <v>7</v>
+      </c>
+      <c r="G9" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" t="n">
+        <v>7</v>
+      </c>
+      <c r="I9" t="n">
         <v>116877349</v>
       </c>
-      <c r="G9" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H9" t="inlineStr">
+      <c r="J9" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>Bank Of America Na</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>COWE-20-001539</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>Jacques</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>Gregoire</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>2150 NW 30 WAY</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>33311-3237</t>
         </is>
@@ -1082,58 +1169,67 @@
         <v>8</v>
       </c>
       <c r="F10" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8</v>
+      </c>
+      <c r="H10" t="n">
+        <v>8</v>
+      </c>
+      <c r="I10" t="n">
         <v>116877473</v>
       </c>
-      <c r="G10" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H10" t="inlineStr">
+      <c r="J10" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>Midland Credit Management Inc</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>COCE-20-016173</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>Sanley</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr">
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr">
         <is>
           <t>Etienne</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>307 NW 1 AVENUE #908</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="U10" t="inlineStr">
         <is>
           <t>33301-1021</t>
         </is>
@@ -1156,62 +1252,71 @@
         <v>9</v>
       </c>
       <c r="F11" t="n">
+        <v>9</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9</v>
+      </c>
+      <c r="H11" t="n">
+        <v>9</v>
+      </c>
+      <c r="I11" t="n">
         <v>116877491</v>
       </c>
-      <c r="G11" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H11" t="inlineStr">
+      <c r="J11" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>COCE-20-008398</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>Carlos</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>Londono</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>11433 NW 10 STREET</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>PEMBROKE PINES</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr">
+      <c r="U11" t="inlineStr">
         <is>
           <t>33026-3832</t>
         </is>
@@ -1234,58 +1339,67 @@
         <v>10</v>
       </c>
       <c r="F12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" t="n">
+        <v>10</v>
+      </c>
+      <c r="H12" t="n">
+        <v>10</v>
+      </c>
+      <c r="I12" t="n">
         <v>116877510</v>
       </c>
-      <c r="G12" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H12" t="inlineStr">
+      <c r="J12" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>COCE-20-024842</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>Stephanie</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr">
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr">
         <is>
           <t>Zuluaga</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>4001 NW 34 STREET #201</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="S12" t="inlineStr">
         <is>
           <t>LAUDERDALE LAKES</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr">
+      <c r="U12" t="inlineStr">
         <is>
           <t>33319-5764</t>
         </is>
@@ -1308,58 +1422,67 @@
         <v>11</v>
       </c>
       <c r="F13" t="n">
+        <v>11</v>
+      </c>
+      <c r="G13" t="n">
+        <v>11</v>
+      </c>
+      <c r="H13" t="n">
+        <v>11</v>
+      </c>
+      <c r="I13" t="n">
         <v>116877515</v>
       </c>
-      <c r="G13" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H13" t="inlineStr">
+      <c r="J13" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>COSO-20-002324</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>Johanna</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr">
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr">
         <is>
           <t>Nunez</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="R13" t="inlineStr">
         <is>
           <t>11201 SW 55 STREET #307</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="S13" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R13" t="n">
+      <c r="U13" t="n">
         <v>33025</v>
       </c>
     </row>
@@ -1380,58 +1503,67 @@
         <v>12</v>
       </c>
       <c r="F14" t="n">
+        <v>12</v>
+      </c>
+      <c r="G14" t="n">
+        <v>12</v>
+      </c>
+      <c r="H14" t="n">
+        <v>12</v>
+      </c>
+      <c r="I14" t="n">
         <v>116877519</v>
       </c>
-      <c r="G14" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H14" t="inlineStr">
+      <c r="J14" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>COCE-20-024861</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>Gabriel</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr">
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>Vermenton</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="R14" t="inlineStr">
         <is>
           <t>5078 S UNIVERSITY DRIVE</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="S14" t="inlineStr">
         <is>
           <t>DAVIE</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="T14" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
+      <c r="U14" t="inlineStr">
         <is>
           <t>33328-4509</t>
         </is>
@@ -1454,58 +1586,67 @@
         <v>13</v>
       </c>
       <c r="F15" t="n">
+        <v>13</v>
+      </c>
+      <c r="G15" t="n">
+        <v>13</v>
+      </c>
+      <c r="H15" t="n">
+        <v>13</v>
+      </c>
+      <c r="I15" t="n">
         <v>116877641</v>
       </c>
-      <c r="G15" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H15" t="inlineStr">
+      <c r="J15" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>Cavalry Spv I LLC</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>COCE-20-001654</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>Valycia</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr">
         <is>
           <t>Cureton</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="R15" t="inlineStr">
         <is>
           <t>10140 NW 4 COURT</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="S15" t="inlineStr">
         <is>
           <t>PEMBROKE PINES</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
+      <c r="T15" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr">
+      <c r="U15" t="inlineStr">
         <is>
           <t>33026-3977</t>
         </is>
@@ -1528,58 +1669,67 @@
         <v>14</v>
       </c>
       <c r="F16" t="n">
+        <v>14</v>
+      </c>
+      <c r="G16" t="n">
+        <v>14</v>
+      </c>
+      <c r="H16" t="n">
+        <v>14</v>
+      </c>
+      <c r="I16" t="n">
         <v>116877648</v>
       </c>
-      <c r="G16" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H16" t="inlineStr">
+      <c r="J16" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>COCE-20-008634</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>Ayed</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr">
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr">
         <is>
           <t>Mohammed</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="R16" t="inlineStr">
         <is>
           <t>4125 NW 65 AVENUE</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="S16" t="inlineStr">
         <is>
           <t>CORAL SPRINGS</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
+      <c r="U16" t="inlineStr">
         <is>
           <t>33067-3037</t>
         </is>
@@ -1602,62 +1752,71 @@
         <v>15</v>
       </c>
       <c r="F17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G17" t="n">
+        <v>15</v>
+      </c>
+      <c r="H17" t="n">
+        <v>15</v>
+      </c>
+      <c r="I17" t="n">
         <v>116877675</v>
       </c>
-      <c r="G17" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H17" t="inlineStr">
+      <c r="J17" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="N17" t="inlineStr">
         <is>
           <t>COCE-20-008636</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="O17" t="inlineStr">
         <is>
           <t>Marica</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="P17" t="inlineStr">
         <is>
           <t>Christie</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
+      <c r="Q17" t="inlineStr">
         <is>
           <t>Hamilton</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
+      <c r="R17" t="inlineStr">
         <is>
           <t>6058 SW 19 STREET</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
+      <c r="S17" t="inlineStr">
         <is>
           <t>NORTH LAUDERDALE</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
+      <c r="T17" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr">
+      <c r="U17" t="inlineStr">
         <is>
           <t>33068-4613</t>
         </is>
@@ -1680,42 +1839,51 @@
         <v>16</v>
       </c>
       <c r="F18" t="n">
+        <v>16</v>
+      </c>
+      <c r="G18" t="n">
+        <v>16</v>
+      </c>
+      <c r="H18" t="n">
+        <v>16</v>
+      </c>
+      <c r="I18" t="n">
         <v>116877677</v>
       </c>
-      <c r="G18" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H18" t="inlineStr">
+      <c r="J18" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>Petersburg Hospital Company LLC</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>CONO-17-002495</t>
-        </is>
-      </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Leila</t>
+          <t>FJ</t>
         </is>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
+          <t>CONO-17-002495</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Leila</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr">
+        <is>
           <t>Mazzone</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1734,58 +1902,67 @@
         <v>17</v>
       </c>
       <c r="F19" t="n">
+        <v>17</v>
+      </c>
+      <c r="G19" t="n">
+        <v>17</v>
+      </c>
+      <c r="H19" t="n">
+        <v>17</v>
+      </c>
+      <c r="I19" t="n">
         <v>116877679</v>
       </c>
-      <c r="G19" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H19" t="inlineStr">
+      <c r="J19" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>Cavalry Spv I LLC</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="N19" t="inlineStr">
         <is>
           <t>COCE-20-008435</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="O19" t="inlineStr">
         <is>
           <t>Murry</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr">
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr">
         <is>
           <t>Schlessinger</t>
         </is>
       </c>
-      <c r="O19" t="inlineStr">
+      <c r="R19" t="inlineStr">
         <is>
           <t>2521 NW 104 AVE #207</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
+      <c r="S19" t="inlineStr">
         <is>
           <t>SUNRISE</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
+      <c r="T19" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr">
+      <c r="U19" t="inlineStr">
         <is>
           <t>33322-6348</t>
         </is>
@@ -1808,58 +1985,67 @@
         <v>18</v>
       </c>
       <c r="F20" t="n">
+        <v>18</v>
+      </c>
+      <c r="G20" t="n">
+        <v>18</v>
+      </c>
+      <c r="H20" t="n">
+        <v>18</v>
+      </c>
+      <c r="I20" t="n">
         <v>116877684</v>
       </c>
-      <c r="G20" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H20" t="inlineStr">
+      <c r="J20" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>COCE-20-008403</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="O20" t="inlineStr">
         <is>
           <t>Keith</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr">
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr">
         <is>
           <t>Salomon</t>
         </is>
       </c>
-      <c r="O20" t="inlineStr">
+      <c r="R20" t="inlineStr">
         <is>
           <t>6550 SW 27 PLACE</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr">
+      <c r="S20" t="inlineStr">
         <is>
           <t>MIRAMAR</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr">
+      <c r="T20" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr">
+      <c r="U20" t="inlineStr">
         <is>
           <t>33023-3838</t>
         </is>
@@ -1882,46 +2068,55 @@
         <v>19</v>
       </c>
       <c r="F21" t="n">
+        <v>19</v>
+      </c>
+      <c r="G21" t="n">
+        <v>19</v>
+      </c>
+      <c r="H21" t="n">
+        <v>19</v>
+      </c>
+      <c r="I21" t="n">
         <v>116877690</v>
       </c>
-      <c r="G21" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H21" t="inlineStr">
+      <c r="J21" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>Cavalry Spv I LLC</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr">
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
         <is>
           <t>COWE-17-004647</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr">
+      <c r="O21" t="inlineStr">
         <is>
           <t>Franklin</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="P21" t="inlineStr">
         <is>
           <t>J</t>
         </is>
       </c>
-      <c r="N21" t="inlineStr">
+      <c r="Q21" t="inlineStr">
         <is>
           <t>Barahona</t>
         </is>
       </c>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1940,62 +2135,71 @@
         <v>20</v>
       </c>
       <c r="F22" t="n">
+        <v>20</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" t="n">
+        <v>20</v>
+      </c>
+      <c r="I22" t="n">
         <v>116877691</v>
       </c>
-      <c r="G22" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H22" t="inlineStr">
+      <c r="J22" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="N22" t="inlineStr">
         <is>
           <t>COCE-20-008605</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
+      <c r="O22" t="inlineStr">
         <is>
           <t>Ayanna</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="P22" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="N22" t="inlineStr">
+      <c r="Q22" t="inlineStr">
         <is>
           <t>Streete</t>
         </is>
       </c>
-      <c r="O22" t="inlineStr">
+      <c r="R22" t="inlineStr">
         <is>
           <t>7715 YARDLEY DRIVE #109</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr">
+      <c r="S22" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
+      <c r="T22" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr">
+      <c r="U22" t="inlineStr">
         <is>
           <t>33321-0859</t>
         </is>
@@ -2018,58 +2222,67 @@
         <v>21</v>
       </c>
       <c r="F23" t="n">
+        <v>21</v>
+      </c>
+      <c r="G23" t="n">
+        <v>21</v>
+      </c>
+      <c r="H23" t="n">
+        <v>21</v>
+      </c>
+      <c r="I23" t="n">
         <v>116877693</v>
       </c>
-      <c r="G23" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H23" t="inlineStr">
+      <c r="J23" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>Midland Credit Management Inc</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
+      <c r="N23" t="inlineStr">
         <is>
           <t>COCE-20-020540</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
+      <c r="O23" t="inlineStr">
         <is>
           <t>Robert</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr">
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
         <is>
           <t>Knapp</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr">
+      <c r="R23" t="inlineStr">
         <is>
           <t>1570 NW 128 DRIVE #110</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr">
+      <c r="S23" t="inlineStr">
         <is>
           <t>SUNRISE</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
+      <c r="T23" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr">
+      <c r="U23" t="inlineStr">
         <is>
           <t>33323-5215</t>
         </is>
@@ -2092,58 +2305,67 @@
         <v>22</v>
       </c>
       <c r="F24" t="n">
+        <v>22</v>
+      </c>
+      <c r="G24" t="n">
+        <v>22</v>
+      </c>
+      <c r="H24" t="n">
+        <v>22</v>
+      </c>
+      <c r="I24" t="n">
         <v>116877708</v>
       </c>
-      <c r="G24" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H24" t="inlineStr">
+      <c r="J24" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="N24" t="inlineStr">
         <is>
           <t>COCE-20-024840</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
+      <c r="O24" t="inlineStr">
         <is>
           <t>Jonathan</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr">
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr">
         <is>
           <t>Duque</t>
         </is>
       </c>
-      <c r="O24" t="inlineStr">
+      <c r="R24" t="inlineStr">
         <is>
           <t>17404 SW 31 COURT</t>
         </is>
       </c>
-      <c r="P24" t="inlineStr">
+      <c r="S24" t="inlineStr">
         <is>
           <t>MIRAMAR</t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr">
+      <c r="T24" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R24" t="inlineStr">
+      <c r="U24" t="inlineStr">
         <is>
           <t>33029-5588</t>
         </is>
@@ -2166,58 +2388,67 @@
         <v>23</v>
       </c>
       <c r="F25" t="n">
+        <v>23</v>
+      </c>
+      <c r="G25" t="n">
+        <v>23</v>
+      </c>
+      <c r="H25" t="n">
+        <v>23</v>
+      </c>
+      <c r="I25" t="n">
         <v>116877709</v>
       </c>
-      <c r="G25" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H25" t="inlineStr">
+      <c r="J25" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>Cavalry Spv I LLC</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="N25" t="inlineStr">
         <is>
           <t>COCE-20-001491</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
+      <c r="O25" t="inlineStr">
         <is>
           <t>Rachel</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr">
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr">
         <is>
           <t>Lacroix</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="R25" t="inlineStr">
         <is>
           <t>8837 ANDORA DRIVE</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr">
+      <c r="S25" t="inlineStr">
         <is>
           <t>MIRAMAR</t>
         </is>
       </c>
-      <c r="Q25" t="inlineStr">
+      <c r="T25" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R25" t="inlineStr">
+      <c r="U25" t="inlineStr">
         <is>
           <t>33025-2558</t>
         </is>
@@ -2240,58 +2471,67 @@
         <v>24</v>
       </c>
       <c r="F26" t="n">
+        <v>24</v>
+      </c>
+      <c r="G26" t="n">
+        <v>24</v>
+      </c>
+      <c r="H26" t="n">
+        <v>24</v>
+      </c>
+      <c r="I26" t="n">
         <v>116877721</v>
       </c>
-      <c r="G26" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H26" t="inlineStr">
+      <c r="J26" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
+      <c r="N26" t="inlineStr">
         <is>
           <t>COSO-18-007361</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
+      <c r="O26" t="inlineStr">
         <is>
           <t>Joseph</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr">
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr">
         <is>
           <t>Jean</t>
         </is>
       </c>
-      <c r="O26" t="inlineStr">
+      <c r="R26" t="inlineStr">
         <is>
           <t>15819 NW 11 STREET</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr">
+      <c r="S26" t="inlineStr">
         <is>
           <t>PEMBROKE PINES</t>
         </is>
       </c>
-      <c r="Q26" t="inlineStr">
+      <c r="T26" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R26" t="n">
+      <c r="U26" t="n">
         <v>33028</v>
       </c>
     </row>
@@ -2312,58 +2552,67 @@
         <v>25</v>
       </c>
       <c r="F27" t="n">
+        <v>25</v>
+      </c>
+      <c r="G27" t="n">
+        <v>25</v>
+      </c>
+      <c r="H27" t="n">
+        <v>25</v>
+      </c>
+      <c r="I27" t="n">
         <v>116877726</v>
       </c>
-      <c r="G27" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H27" t="inlineStr">
+      <c r="J27" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="N27" t="inlineStr">
         <is>
           <t>COCE-20-024782</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr">
+      <c r="O27" t="inlineStr">
         <is>
           <t>Nicole</t>
         </is>
       </c>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr">
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr">
         <is>
           <t>Kuhar</t>
         </is>
       </c>
-      <c r="O27" t="inlineStr">
+      <c r="R27" t="inlineStr">
         <is>
           <t>4840 NE 5 AVENUE</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr">
+      <c r="S27" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="Q27" t="inlineStr">
+      <c r="T27" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R27" t="inlineStr">
+      <c r="U27" t="inlineStr">
         <is>
           <t>33334-2322</t>
         </is>
@@ -2386,62 +2635,71 @@
         <v>26</v>
       </c>
       <c r="F28" t="n">
+        <v>26</v>
+      </c>
+      <c r="G28" t="n">
+        <v>26</v>
+      </c>
+      <c r="H28" t="n">
+        <v>26</v>
+      </c>
+      <c r="I28" t="n">
         <v>116877737</v>
       </c>
-      <c r="G28" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H28" t="inlineStr">
+      <c r="J28" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
+      <c r="N28" t="inlineStr">
         <is>
           <t>COCE-20-008401</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr">
+      <c r="O28" t="inlineStr">
         <is>
           <t>Noah</t>
         </is>
       </c>
-      <c r="M28" t="inlineStr">
+      <c r="P28" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="N28" t="inlineStr">
+      <c r="Q28" t="inlineStr">
         <is>
           <t>Jones</t>
         </is>
       </c>
-      <c r="O28" t="inlineStr">
+      <c r="R28" t="inlineStr">
         <is>
           <t>7466 NW 47 PLACE</t>
         </is>
       </c>
-      <c r="P28" t="inlineStr">
+      <c r="S28" t="inlineStr">
         <is>
           <t>LAUDERHILL</t>
         </is>
       </c>
-      <c r="Q28" t="inlineStr">
+      <c r="T28" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R28" t="inlineStr">
+      <c r="U28" t="inlineStr">
         <is>
           <t>33319-3416</t>
         </is>
@@ -2464,58 +2722,67 @@
         <v>27</v>
       </c>
       <c r="F29" t="n">
+        <v>27</v>
+      </c>
+      <c r="G29" t="n">
+        <v>27</v>
+      </c>
+      <c r="H29" t="n">
+        <v>27</v>
+      </c>
+      <c r="I29" t="n">
         <v>116877742</v>
       </c>
-      <c r="G29" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H29" t="inlineStr">
+      <c r="J29" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>Capital One Bank Usa</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="N29" t="inlineStr">
         <is>
           <t>COCE-18-027671</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
+      <c r="O29" t="inlineStr">
         <is>
           <t>Stefanie</t>
         </is>
       </c>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr">
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr">
         <is>
           <t>Rodriguez</t>
         </is>
       </c>
-      <c r="O29" t="inlineStr">
+      <c r="R29" t="inlineStr">
         <is>
           <t>1141 NE 17 AVENUE #3</t>
         </is>
       </c>
-      <c r="P29" t="inlineStr">
+      <c r="S29" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="Q29" t="inlineStr">
+      <c r="T29" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R29" t="n">
+      <c r="U29" t="n">
         <v>33304</v>
       </c>
     </row>
@@ -2536,62 +2803,71 @@
         <v>28</v>
       </c>
       <c r="F30" t="n">
+        <v>28</v>
+      </c>
+      <c r="G30" t="n">
+        <v>28</v>
+      </c>
+      <c r="H30" t="n">
+        <v>28</v>
+      </c>
+      <c r="I30" t="n">
         <v>116877760</v>
       </c>
-      <c r="G30" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H30" t="inlineStr">
+      <c r="J30" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>Wynmoor Nassau Village Assn Inc</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="N30" t="inlineStr">
         <is>
           <t>CONO-20-013473</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr">
+      <c r="O30" t="inlineStr">
         <is>
           <t>Richard</t>
         </is>
       </c>
-      <c r="M30" t="inlineStr">
+      <c r="P30" t="inlineStr">
         <is>
           <t>Jr</t>
         </is>
       </c>
-      <c r="N30" t="inlineStr">
+      <c r="Q30" t="inlineStr">
         <is>
           <t>Udovich</t>
         </is>
       </c>
-      <c r="O30" t="inlineStr">
+      <c r="R30" t="inlineStr">
         <is>
           <t>2710 NASSAU BEND #F1</t>
         </is>
       </c>
-      <c r="P30" t="inlineStr">
+      <c r="S30" t="inlineStr">
         <is>
           <t>COCONUT CREEK</t>
         </is>
       </c>
-      <c r="Q30" t="inlineStr">
+      <c r="T30" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R30" t="n">
+      <c r="U30" t="n">
         <v>33066</v>
       </c>
     </row>
@@ -2612,58 +2888,67 @@
         <v>29</v>
       </c>
       <c r="F31" t="n">
+        <v>29</v>
+      </c>
+      <c r="G31" t="n">
+        <v>29</v>
+      </c>
+      <c r="H31" t="n">
+        <v>29</v>
+      </c>
+      <c r="I31" t="n">
         <v>116877785</v>
       </c>
-      <c r="G31" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H31" t="inlineStr">
+      <c r="J31" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr">
+      <c r="N31" t="inlineStr">
         <is>
           <t>COCE-20-009469</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr">
+      <c r="O31" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr">
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr">
         <is>
           <t>Hughes</t>
         </is>
       </c>
-      <c r="O31" t="inlineStr">
+      <c r="R31" t="inlineStr">
         <is>
           <t>2544 NW 99 AVENUE</t>
         </is>
       </c>
-      <c r="P31" t="inlineStr">
+      <c r="S31" t="inlineStr">
         <is>
           <t>CORAL SPRINGS</t>
         </is>
       </c>
-      <c r="Q31" t="inlineStr">
+      <c r="T31" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R31" t="inlineStr">
+      <c r="U31" t="inlineStr">
         <is>
           <t>33065-6207</t>
         </is>
@@ -2686,58 +2971,67 @@
         <v>30</v>
       </c>
       <c r="F32" t="n">
+        <v>30</v>
+      </c>
+      <c r="G32" t="n">
+        <v>30</v>
+      </c>
+      <c r="H32" t="n">
+        <v>30</v>
+      </c>
+      <c r="I32" t="n">
         <v>116877826</v>
       </c>
-      <c r="G32" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H32" t="inlineStr">
+      <c r="J32" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr">
+      <c r="N32" t="inlineStr">
         <is>
           <t>COCE-20-015574</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
+      <c r="O32" t="inlineStr">
         <is>
           <t>Jackie</t>
         </is>
       </c>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr">
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr">
         <is>
           <t>Alexander</t>
         </is>
       </c>
-      <c r="O32" t="inlineStr">
+      <c r="R32" t="inlineStr">
         <is>
           <t>1626 S 17 AVENUE</t>
         </is>
       </c>
-      <c r="P32" t="inlineStr">
+      <c r="S32" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="Q32" t="inlineStr">
+      <c r="T32" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R32" t="inlineStr">
+      <c r="U32" t="inlineStr">
         <is>
           <t>33020-6535</t>
         </is>
@@ -2760,58 +3054,67 @@
         <v>31</v>
       </c>
       <c r="F33" t="n">
+        <v>31</v>
+      </c>
+      <c r="G33" t="n">
+        <v>31</v>
+      </c>
+      <c r="H33" t="n">
+        <v>31</v>
+      </c>
+      <c r="I33" t="n">
         <v>116877840</v>
       </c>
-      <c r="G33" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H33" t="inlineStr">
+      <c r="J33" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr">
+      <c r="N33" t="inlineStr">
         <is>
           <t>COCE-20-015582</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr">
+      <c r="O33" t="inlineStr">
         <is>
           <t>Jennifer</t>
         </is>
       </c>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr">
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr">
         <is>
           <t>Matos</t>
         </is>
       </c>
-      <c r="O33" t="inlineStr">
+      <c r="R33" t="inlineStr">
         <is>
           <t>3777 NW 78 AVENUE #11F</t>
         </is>
       </c>
-      <c r="P33" t="inlineStr">
+      <c r="S33" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="Q33" t="inlineStr">
+      <c r="T33" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R33" t="inlineStr">
+      <c r="U33" t="inlineStr">
         <is>
           <t>33024-8342</t>
         </is>
@@ -2834,58 +3137,67 @@
         <v>32</v>
       </c>
       <c r="F34" t="n">
+        <v>32</v>
+      </c>
+      <c r="G34" t="n">
+        <v>32</v>
+      </c>
+      <c r="H34" t="n">
+        <v>32</v>
+      </c>
+      <c r="I34" t="n">
         <v>116877868</v>
       </c>
-      <c r="G34" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H34" t="inlineStr">
+      <c r="J34" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>Tidewater Finance Company</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr">
+      <c r="N34" t="inlineStr">
         <is>
           <t>COCE-20-023825</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr">
+      <c r="O34" t="inlineStr">
         <is>
           <t>Louisne</t>
         </is>
       </c>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr">
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr">
         <is>
           <t>Joseph</t>
         </is>
       </c>
-      <c r="O34" t="inlineStr">
+      <c r="R34" t="inlineStr">
         <is>
           <t>6391 SW 34 STREET</t>
         </is>
       </c>
-      <c r="P34" t="inlineStr">
+      <c r="S34" t="inlineStr">
         <is>
           <t>MIRAMAR</t>
         </is>
       </c>
-      <c r="Q34" t="inlineStr">
+      <c r="T34" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R34" t="n">
+      <c r="U34" t="n">
         <v>33023</v>
       </c>
     </row>
@@ -2906,58 +3218,67 @@
         <v>33</v>
       </c>
       <c r="F35" t="n">
+        <v>33</v>
+      </c>
+      <c r="G35" t="n">
+        <v>33</v>
+      </c>
+      <c r="H35" t="n">
+        <v>33</v>
+      </c>
+      <c r="I35" t="n">
         <v>116877871</v>
       </c>
-      <c r="G35" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H35" t="inlineStr">
+      <c r="J35" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>Platinum Public Adjusters Inc</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr">
+      <c r="N35" t="inlineStr">
         <is>
           <t>COCE-20-009956</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr">
+      <c r="O35" t="inlineStr">
         <is>
           <t>Alvin</t>
         </is>
       </c>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr">
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr">
         <is>
           <t>Gray</t>
         </is>
       </c>
-      <c r="O35" t="inlineStr">
+      <c r="R35" t="inlineStr">
         <is>
           <t>3174 NW 43 STREET</t>
         </is>
       </c>
-      <c r="P35" t="inlineStr">
+      <c r="S35" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="Q35" t="inlineStr">
+      <c r="T35" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R35" t="n">
+      <c r="U35" t="n">
         <v>33309</v>
       </c>
     </row>
@@ -2978,58 +3299,67 @@
         <v>34</v>
       </c>
       <c r="F36" t="n">
+        <v>34</v>
+      </c>
+      <c r="G36" t="n">
+        <v>34</v>
+      </c>
+      <c r="H36" t="n">
+        <v>34</v>
+      </c>
+      <c r="I36" t="n">
         <v>116877906</v>
       </c>
-      <c r="G36" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H36" t="inlineStr">
+      <c r="J36" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>Unifund Ccr LLC</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr">
+      <c r="N36" t="inlineStr">
         <is>
           <t>COCE-20-015657</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr">
+      <c r="O36" t="inlineStr">
         <is>
           <t>Julia</t>
         </is>
       </c>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr">
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr">
         <is>
           <t>Mizaur</t>
         </is>
       </c>
-      <c r="O36" t="inlineStr">
+      <c r="R36" t="inlineStr">
         <is>
           <t>2336 TAFT STREET</t>
         </is>
       </c>
-      <c r="P36" t="inlineStr">
+      <c r="S36" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="Q36" t="inlineStr">
+      <c r="T36" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R36" t="n">
+      <c r="U36" t="n">
         <v>33020</v>
       </c>
     </row>
@@ -3050,58 +3380,67 @@
         <v>35</v>
       </c>
       <c r="F37" t="n">
+        <v>35</v>
+      </c>
+      <c r="G37" t="n">
+        <v>35</v>
+      </c>
+      <c r="H37" t="n">
+        <v>35</v>
+      </c>
+      <c r="I37" t="n">
         <v>116877910</v>
       </c>
-      <c r="G37" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H37" t="inlineStr">
+      <c r="J37" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr">
+      <c r="N37" t="inlineStr">
         <is>
           <t>COCE-20-008433</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr">
+      <c r="O37" t="inlineStr">
         <is>
           <t>Carmen</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr">
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr">
         <is>
           <t>Mora</t>
         </is>
       </c>
-      <c r="O37" t="inlineStr">
+      <c r="R37" t="inlineStr">
         <is>
           <t>3917 E SHORE ROAD</t>
         </is>
       </c>
-      <c r="P37" t="inlineStr">
+      <c r="S37" t="inlineStr">
         <is>
           <t>MIRAMAR</t>
         </is>
       </c>
-      <c r="Q37" t="inlineStr">
+      <c r="T37" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R37" t="inlineStr">
+      <c r="U37" t="inlineStr">
         <is>
           <t>33023-4959</t>
         </is>
@@ -3124,58 +3463,67 @@
         <v>36</v>
       </c>
       <c r="F38" t="n">
+        <v>36</v>
+      </c>
+      <c r="G38" t="n">
+        <v>36</v>
+      </c>
+      <c r="H38" t="n">
+        <v>36</v>
+      </c>
+      <c r="I38" t="n">
         <v>116877929</v>
       </c>
-      <c r="G38" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H38" t="inlineStr">
+      <c r="J38" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K38" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K38" t="inlineStr">
+      <c r="N38" t="inlineStr">
         <is>
           <t>COCE-20-008434</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr">
+      <c r="O38" t="inlineStr">
         <is>
           <t>Andres</t>
         </is>
       </c>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr">
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr">
         <is>
           <t>Sanchez</t>
         </is>
       </c>
-      <c r="O38" t="inlineStr">
+      <c r="R38" t="inlineStr">
         <is>
           <t>1425 SAINT GABRIELLE LANE</t>
         </is>
       </c>
-      <c r="P38" t="inlineStr">
+      <c r="S38" t="inlineStr">
         <is>
           <t>WESTON</t>
         </is>
       </c>
-      <c r="Q38" t="inlineStr">
+      <c r="T38" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R38" t="inlineStr">
+      <c r="U38" t="inlineStr">
         <is>
           <t>33326-4029</t>
         </is>
@@ -3198,42 +3546,51 @@
         <v>37</v>
       </c>
       <c r="F39" t="n">
+        <v>37</v>
+      </c>
+      <c r="G39" t="n">
+        <v>37</v>
+      </c>
+      <c r="H39" t="n">
+        <v>37</v>
+      </c>
+      <c r="I39" t="n">
         <v>116878464</v>
       </c>
-      <c r="G39" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H39" t="inlineStr">
+      <c r="J39" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>Cach LLC</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr"/>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>CONO-13-009293</t>
-        </is>
-      </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Marie</t>
+          <t>FJ</t>
         </is>
       </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr">
         <is>
+          <t>CONO-13-009293</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Marie</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr">
+        <is>
           <t>Stphard</t>
         </is>
       </c>
-      <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr"/>
+      <c r="U39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -3252,42 +3609,51 @@
         <v>38</v>
       </c>
       <c r="F40" t="n">
+        <v>38</v>
+      </c>
+      <c r="G40" t="n">
+        <v>38</v>
+      </c>
+      <c r="H40" t="n">
+        <v>38</v>
+      </c>
+      <c r="I40" t="n">
         <v>116878760</v>
       </c>
-      <c r="G40" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H40" t="inlineStr">
+      <c r="J40" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>Arrow Financial Services LLC</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr"/>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>COWE-10-018019</t>
-        </is>
-      </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Corence</t>
+          <t>FJ</t>
         </is>
       </c>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr">
         <is>
+          <t>COWE-10-018019</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Corence</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr">
+        <is>
           <t>Chisholm</t>
         </is>
       </c>
-      <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr"/>
+      <c r="U40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -3306,46 +3672,55 @@
         <v>39</v>
       </c>
       <c r="F41" t="n">
+        <v>39</v>
+      </c>
+      <c r="G41" t="n">
+        <v>39</v>
+      </c>
+      <c r="H41" t="n">
+        <v>39</v>
+      </c>
+      <c r="I41" t="n">
         <v>116878793</v>
       </c>
-      <c r="G41" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H41" t="inlineStr">
+      <c r="J41" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>Progressive Select Ins Co</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr"/>
-      <c r="K41" t="inlineStr">
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr">
         <is>
           <t>COWE-20-010184</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr">
+      <c r="O41" t="inlineStr">
         <is>
           <t>Dakota</t>
         </is>
       </c>
-      <c r="M41" t="inlineStr">
+      <c r="P41" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="N41" t="inlineStr">
+      <c r="Q41" t="inlineStr">
         <is>
           <t>Mcquiston</t>
         </is>
       </c>
-      <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr"/>
-      <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -3364,46 +3739,55 @@
         <v>40</v>
       </c>
       <c r="F42" t="n">
+        <v>40</v>
+      </c>
+      <c r="G42" t="n">
+        <v>40</v>
+      </c>
+      <c r="H42" t="n">
+        <v>40</v>
+      </c>
+      <c r="I42" t="n">
         <v>116878798</v>
       </c>
-      <c r="G42" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H42" t="inlineStr">
+      <c r="J42" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>Progressive Select Ins Co</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr">
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr">
         <is>
           <t>COWE-20-010052</t>
         </is>
       </c>
-      <c r="L42" t="inlineStr">
+      <c r="O42" t="inlineStr">
         <is>
           <t>Jarvierre</t>
         </is>
       </c>
-      <c r="M42" t="inlineStr">
+      <c r="P42" t="inlineStr">
         <is>
           <t>Deontaye</t>
         </is>
       </c>
-      <c r="N42" t="inlineStr">
+      <c r="Q42" t="inlineStr">
         <is>
           <t>Rogers</t>
         </is>
       </c>
-      <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr"/>
-      <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -3422,62 +3806,71 @@
         <v>41</v>
       </c>
       <c r="F43" t="n">
+        <v>41</v>
+      </c>
+      <c r="G43" t="n">
+        <v>41</v>
+      </c>
+      <c r="H43" t="n">
+        <v>41</v>
+      </c>
+      <c r="I43" t="n">
         <v>116878808</v>
       </c>
-      <c r="G43" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H43" t="inlineStr">
+      <c r="J43" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K43" t="inlineStr">
         <is>
           <t>Progressive Select Insurance Company</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K43" t="inlineStr">
+      <c r="N43" t="inlineStr">
         <is>
           <t>COWE-20-020167</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr">
+      <c r="O43" t="inlineStr">
         <is>
           <t>Julio</t>
         </is>
       </c>
-      <c r="M43" t="inlineStr">
+      <c r="P43" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="N43" t="inlineStr">
+      <c r="Q43" t="inlineStr">
         <is>
           <t>Rojas</t>
         </is>
       </c>
-      <c r="O43" t="inlineStr">
+      <c r="R43" t="inlineStr">
         <is>
           <t>7440 SW 36 STREET</t>
         </is>
       </c>
-      <c r="P43" t="inlineStr">
+      <c r="S43" t="inlineStr">
         <is>
           <t>DAVIE</t>
         </is>
       </c>
-      <c r="Q43" t="inlineStr">
+      <c r="T43" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R43" t="n">
+      <c r="U43" t="n">
         <v>33314</v>
       </c>
     </row>
@@ -3498,58 +3891,67 @@
         <v>42</v>
       </c>
       <c r="F44" t="n">
+        <v>42</v>
+      </c>
+      <c r="G44" t="n">
+        <v>42</v>
+      </c>
+      <c r="H44" t="n">
+        <v>42</v>
+      </c>
+      <c r="I44" t="n">
         <v>116879076</v>
       </c>
-      <c r="G44" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H44" t="inlineStr">
+      <c r="J44" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>Dept Stores National Bank</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr">
+      <c r="N44" t="inlineStr">
         <is>
           <t>COWE-20-005199</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
+      <c r="O44" t="inlineStr">
         <is>
           <t>Anee</t>
         </is>
       </c>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr">
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr">
         <is>
           <t>Villalba</t>
         </is>
       </c>
-      <c r="O44" t="inlineStr">
+      <c r="R44" t="inlineStr">
         <is>
           <t>121 NW 21 STREET</t>
         </is>
       </c>
-      <c r="P44" t="inlineStr">
+      <c r="S44" t="inlineStr">
         <is>
           <t>POMPANO BEACH</t>
         </is>
       </c>
-      <c r="Q44" t="inlineStr">
+      <c r="T44" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R44" t="n">
+      <c r="U44" t="n">
         <v>33060</v>
       </c>
     </row>
@@ -3570,46 +3972,55 @@
         <v>43</v>
       </c>
       <c r="F45" t="n">
+        <v>43</v>
+      </c>
+      <c r="G45" t="n">
+        <v>43</v>
+      </c>
+      <c r="H45" t="n">
+        <v>43</v>
+      </c>
+      <c r="I45" t="n">
         <v>116879414</v>
       </c>
-      <c r="G45" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H45" t="inlineStr">
+      <c r="J45" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>Aig Enterprise Corp</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="inlineStr">
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr">
         <is>
           <t>CONO-20-019654</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr">
+      <c r="O45" t="inlineStr">
         <is>
           <t>Robertson</t>
         </is>
       </c>
-      <c r="M45" t="inlineStr">
+      <c r="P45" t="inlineStr">
         <is>
           <t>Marcus</t>
         </is>
       </c>
-      <c r="N45" t="inlineStr">
+      <c r="Q45" t="inlineStr">
         <is>
           <t>Dean</t>
         </is>
       </c>
-      <c r="O45" t="inlineStr"/>
-      <c r="P45" t="inlineStr"/>
-      <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -3628,58 +4039,67 @@
         <v>44</v>
       </c>
       <c r="F46" t="n">
+        <v>44</v>
+      </c>
+      <c r="G46" t="n">
+        <v>44</v>
+      </c>
+      <c r="H46" t="n">
+        <v>44</v>
+      </c>
+      <c r="I46" t="n">
         <v>116879713</v>
       </c>
-      <c r="G46" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H46" t="inlineStr">
+      <c r="J46" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K46" t="inlineStr">
         <is>
           <t>Cavalry Spv I LLC</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr">
+      <c r="N46" t="inlineStr">
         <is>
           <t>COCE-18-014639</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
+      <c r="O46" t="inlineStr">
         <is>
           <t>Marie</t>
         </is>
       </c>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr">
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr">
         <is>
           <t>Chery</t>
         </is>
       </c>
-      <c r="O46" t="inlineStr">
+      <c r="R46" t="inlineStr">
         <is>
           <t>140 NE 27 STREET</t>
         </is>
       </c>
-      <c r="P46" t="inlineStr">
+      <c r="S46" t="inlineStr">
         <is>
           <t>POMPANO BEACH</t>
         </is>
       </c>
-      <c r="Q46" t="inlineStr">
+      <c r="T46" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R46" t="inlineStr">
+      <c r="U46" t="inlineStr">
         <is>
           <t>33064-3628</t>
         </is>
@@ -3702,58 +4122,67 @@
         <v>45</v>
       </c>
       <c r="F47" t="n">
+        <v>45</v>
+      </c>
+      <c r="G47" t="n">
+        <v>45</v>
+      </c>
+      <c r="H47" t="n">
+        <v>45</v>
+      </c>
+      <c r="I47" t="n">
         <v>116879859</v>
       </c>
-      <c r="G47" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H47" t="inlineStr">
+      <c r="J47" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t>Midland Credit Management Inc</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K47" t="inlineStr">
+      <c r="N47" t="inlineStr">
         <is>
           <t>COSO-20-002977</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr">
+      <c r="O47" t="inlineStr">
         <is>
           <t>Dianne</t>
         </is>
       </c>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr">
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr">
         <is>
           <t>Burgess</t>
         </is>
       </c>
-      <c r="O47" t="inlineStr">
+      <c r="R47" t="inlineStr">
         <is>
           <t>1080 S MILITARY TRAIL</t>
         </is>
       </c>
-      <c r="P47" t="inlineStr">
+      <c r="S47" t="inlineStr">
         <is>
           <t>DEERFIELD BEACH</t>
         </is>
       </c>
-      <c r="Q47" t="inlineStr">
+      <c r="T47" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R47" t="inlineStr">
+      <c r="U47" t="inlineStr">
         <is>
           <t>33442-7691</t>
         </is>
@@ -3776,58 +4205,67 @@
         <v>46</v>
       </c>
       <c r="F48" t="n">
+        <v>46</v>
+      </c>
+      <c r="G48" t="n">
+        <v>46</v>
+      </c>
+      <c r="H48" t="n">
+        <v>46</v>
+      </c>
+      <c r="I48" t="n">
         <v>116879870</v>
       </c>
-      <c r="G48" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H48" t="inlineStr">
+      <c r="J48" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K48" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr">
+      <c r="N48" t="inlineStr">
         <is>
           <t>COSO-19-015233</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr">
+      <c r="O48" t="inlineStr">
         <is>
           <t>Donald</t>
         </is>
       </c>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr">
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr">
         <is>
           <t>Siganoff</t>
         </is>
       </c>
-      <c r="O48" t="inlineStr">
+      <c r="R48" t="inlineStr">
         <is>
           <t>661 SE 2 TERRACE</t>
         </is>
       </c>
-      <c r="P48" t="inlineStr">
+      <c r="S48" t="inlineStr">
         <is>
           <t>POMPANO BEACH</t>
         </is>
       </c>
-      <c r="Q48" t="inlineStr">
+      <c r="T48" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R48" t="n">
+      <c r="U48" t="n">
         <v>33060</v>
       </c>
     </row>
@@ -3848,58 +4286,67 @@
         <v>47</v>
       </c>
       <c r="F49" t="n">
+        <v>47</v>
+      </c>
+      <c r="G49" t="n">
+        <v>47</v>
+      </c>
+      <c r="H49" t="n">
+        <v>47</v>
+      </c>
+      <c r="I49" t="n">
         <v>116879890</v>
       </c>
-      <c r="G49" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H49" t="inlineStr">
+      <c r="J49" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr">
+      <c r="N49" t="inlineStr">
         <is>
           <t>COSO-19-010382</t>
         </is>
       </c>
-      <c r="L49" t="inlineStr">
+      <c r="O49" t="inlineStr">
         <is>
           <t>Roberto</t>
         </is>
       </c>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr">
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr">
         <is>
           <t>Martinez</t>
         </is>
       </c>
-      <c r="O49" t="inlineStr">
+      <c r="R49" t="inlineStr">
         <is>
           <t>2840 NE 7 TERRACE</t>
         </is>
       </c>
-      <c r="P49" t="inlineStr">
+      <c r="S49" t="inlineStr">
         <is>
           <t>POMPANO BEACH</t>
         </is>
       </c>
-      <c r="Q49" t="inlineStr">
+      <c r="T49" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R49" t="n">
+      <c r="U49" t="n">
         <v>33064</v>
       </c>
     </row>
@@ -3920,62 +4367,71 @@
         <v>48</v>
       </c>
       <c r="F50" t="n">
+        <v>48</v>
+      </c>
+      <c r="G50" t="n">
+        <v>48</v>
+      </c>
+      <c r="H50" t="n">
+        <v>48</v>
+      </c>
+      <c r="I50" t="n">
         <v>116879960</v>
       </c>
-      <c r="G50" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H50" t="inlineStr">
+      <c r="J50" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K50" t="inlineStr">
         <is>
           <t>Jefferson Capital Systems LLC</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr">
+      <c r="N50" t="inlineStr">
         <is>
           <t>COSO-20-003012</t>
         </is>
       </c>
-      <c r="L50" t="inlineStr">
+      <c r="O50" t="inlineStr">
         <is>
           <t>Jorge</t>
         </is>
       </c>
-      <c r="M50" t="inlineStr">
+      <c r="P50" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="N50" t="inlineStr">
+      <c r="Q50" t="inlineStr">
         <is>
           <t>Dieppa</t>
         </is>
       </c>
-      <c r="O50" t="inlineStr">
+      <c r="R50" t="inlineStr">
         <is>
           <t>7560 POLK STREET</t>
         </is>
       </c>
-      <c r="P50" t="inlineStr">
+      <c r="S50" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="Q50" t="inlineStr">
+      <c r="T50" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R50" t="n">
+      <c r="U50" t="n">
         <v>33024</v>
       </c>
     </row>
@@ -3996,58 +4452,67 @@
         <v>49</v>
       </c>
       <c r="F51" t="n">
+        <v>49</v>
+      </c>
+      <c r="G51" t="n">
+        <v>49</v>
+      </c>
+      <c r="H51" t="n">
+        <v>49</v>
+      </c>
+      <c r="I51" t="n">
         <v>116879961</v>
       </c>
-      <c r="G51" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H51" t="inlineStr">
+      <c r="J51" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K51" t="inlineStr">
         <is>
           <t>Velocity Investments LLC</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr">
+      <c r="N51" t="inlineStr">
         <is>
           <t>COSO-20-009463</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr">
+      <c r="O51" t="inlineStr">
         <is>
           <t>Simon</t>
         </is>
       </c>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr">
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr">
         <is>
           <t>Hernandez</t>
         </is>
       </c>
-      <c r="O51" t="inlineStr">
+      <c r="R51" t="inlineStr">
         <is>
           <t>16711 SAPPHIRE ISLE</t>
         </is>
       </c>
-      <c r="P51" t="inlineStr">
+      <c r="S51" t="inlineStr">
         <is>
           <t>WESTON</t>
         </is>
       </c>
-      <c r="Q51" t="inlineStr">
+      <c r="T51" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R51" t="n">
+      <c r="U51" t="n">
         <v>33331</v>
       </c>
     </row>
@@ -4068,58 +4533,67 @@
         <v>50</v>
       </c>
       <c r="F52" t="n">
+        <v>50</v>
+      </c>
+      <c r="G52" t="n">
+        <v>50</v>
+      </c>
+      <c r="H52" t="n">
+        <v>50</v>
+      </c>
+      <c r="I52" t="n">
         <v>116879962</v>
       </c>
-      <c r="G52" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="H52" t="inlineStr">
+      <c r="J52" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="K52" t="inlineStr">
         <is>
           <t>Velocity Investments LLC</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="K52" t="inlineStr">
+      <c r="N52" t="inlineStr">
         <is>
           <t>COSO-19-006341</t>
         </is>
       </c>
-      <c r="L52" t="inlineStr">
+      <c r="O52" t="inlineStr">
         <is>
           <t>Patricia</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr">
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr">
         <is>
           <t>Garcia</t>
         </is>
       </c>
-      <c r="O52" t="inlineStr">
+      <c r="R52" t="inlineStr">
         <is>
           <t>581 SE 13 STREET #106</t>
         </is>
       </c>
-      <c r="P52" t="inlineStr">
+      <c r="S52" t="inlineStr">
         <is>
           <t>DANIA BEACH</t>
         </is>
       </c>
-      <c r="Q52" t="inlineStr">
+      <c r="T52" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="R52" t="n">
+      <c r="U52" t="n">
         <v>33004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
convert script to exe with icon
Convert file to exe, added icon, added spec file . run pyinstaller ExcelFileUpdater.spec to make changes, also added version to script
</commit_message>
<xml_diff>
--- a/11_20_2020 BRWD FJ RAW.xlsx
+++ b/11_20_2020 BRWD FJ RAW.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U52"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,65 +476,75 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>ClerkFileNumber</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Plaintiff</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Amount $</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Case #</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Def First</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Def MI</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Def Last</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Mailing Address</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>City</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>ST</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Zip</t>
         </is>
@@ -566,46 +576,52 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
         <v>116877265</v>
       </c>
-      <c r="J2" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
           <t>COWE-08-020657</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>Adrianna</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>Jeffery</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -633,58 +649,64 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
         <v>116877266</v>
       </c>
-      <c r="J3" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>Asset Acceptance LLC</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>COWE-06-001326</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Lauren</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr">
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr">
         <is>
           <t>Burley</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>2354 N. Military Trail #210</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>West Palm Beach</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U3" t="n">
+      <c r="W3" t="n">
         <v>33409</v>
       </c>
     </row>
@@ -714,58 +736,64 @@
         <v>2</v>
       </c>
       <c r="I4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" t="n">
         <v>116877268</v>
       </c>
-      <c r="J4" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>Lien Source LLC</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>COSO-20-010813</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>Jean</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr">
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr">
         <is>
           <t>Elie</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>230 NE 61 Street</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>Ft Lauderdale</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="W4" t="inlineStr">
         <is>
           <t>33334-1929</t>
         </is>
@@ -797,58 +825,64 @@
         <v>3</v>
       </c>
       <c r="I5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" t="n">
         <v>116877273</v>
       </c>
-      <c r="J5" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M5" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>COSO-19-007468</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>Humberto</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr">
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr">
         <is>
           <t>Mesa</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>2216 Taft Street</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>Hollywood</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="W5" t="inlineStr">
         <is>
           <t>33020-2641</t>
         </is>
@@ -880,46 +914,52 @@
         <v>4</v>
       </c>
       <c r="I6" t="n">
+        <v>4</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" t="n">
         <v>116877290</v>
       </c>
-      <c r="J6" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M6" t="inlineStr">
         <is>
           <t>Progressive Select Insurance Company</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
           <t>COWE-15-005648</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>Doreen</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>Annmarie</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>Goodgame</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -947,42 +987,48 @@
         <v>5</v>
       </c>
       <c r="I7" t="n">
+        <v>5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>5</v>
+      </c>
+      <c r="K7" t="n">
         <v>116877295</v>
       </c>
-      <c r="J7" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M7" t="inlineStr">
         <is>
           <t>Lago Funding Corp</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
+        <is>
           <t>COSO-17-004512</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>Valerie</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr">
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
         <is>
           <t>Vieux</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1010,58 +1056,64 @@
         <v>6</v>
       </c>
       <c r="I8" t="n">
+        <v>6</v>
+      </c>
+      <c r="J8" t="n">
+        <v>6</v>
+      </c>
+      <c r="K8" t="n">
         <v>116877319</v>
       </c>
-      <c r="J8" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M8" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>COSO-19-003421</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>Calin</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr">
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
         <is>
           <t>Romosan</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>608 S CRESCENT DRIVE</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="U8" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="V8" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U8" t="n">
+      <c r="W8" t="n">
         <v>33021</v>
       </c>
     </row>
@@ -1091,62 +1143,68 @@
         <v>7</v>
       </c>
       <c r="I9" t="n">
+        <v>7</v>
+      </c>
+      <c r="J9" t="n">
+        <v>7</v>
+      </c>
+      <c r="K9" t="n">
         <v>116877349</v>
       </c>
-      <c r="J9" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M9" t="inlineStr">
         <is>
           <t>Bank Of America Na</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>COWE-20-001539</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>Jacques</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>Gregoire</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>2150 NW 30 WAY</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="V9" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr">
+      <c r="W9" t="inlineStr">
         <is>
           <t>33311-3237</t>
         </is>
@@ -1178,58 +1236,64 @@
         <v>8</v>
       </c>
       <c r="I10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J10" t="n">
+        <v>8</v>
+      </c>
+      <c r="K10" t="n">
         <v>116877473</v>
       </c>
-      <c r="J10" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M10" t="inlineStr">
         <is>
           <t>Midland Credit Management Inc</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>COCE-20-016173</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>Sanley</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr">
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
         <is>
           <t>Etienne</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>307 NW 1 AVENUE #908</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="U10" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="V10" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr">
+      <c r="W10" t="inlineStr">
         <is>
           <t>33301-1021</t>
         </is>
@@ -1261,62 +1325,68 @@
         <v>9</v>
       </c>
       <c r="I11" t="n">
+        <v>9</v>
+      </c>
+      <c r="J11" t="n">
+        <v>9</v>
+      </c>
+      <c r="K11" t="n">
         <v>116877491</v>
       </c>
-      <c r="J11" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M11" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>COCE-20-008398</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>Carlos</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>Londono</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>11433 NW 10 STREET</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="U11" t="inlineStr">
         <is>
           <t>PEMBROKE PINES</t>
         </is>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="V11" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr">
+      <c r="W11" t="inlineStr">
         <is>
           <t>33026-3832</t>
         </is>
@@ -1348,58 +1418,64 @@
         <v>10</v>
       </c>
       <c r="I12" t="n">
+        <v>10</v>
+      </c>
+      <c r="J12" t="n">
+        <v>10</v>
+      </c>
+      <c r="K12" t="n">
         <v>116877510</v>
       </c>
-      <c r="J12" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M12" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>COCE-20-024842</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>Stephanie</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr">
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr">
         <is>
           <t>Zuluaga</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>4001 NW 34 STREET #201</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="U12" t="inlineStr">
         <is>
           <t>LAUDERDALE LAKES</t>
         </is>
       </c>
-      <c r="T12" t="inlineStr">
+      <c r="V12" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="W12" t="inlineStr">
         <is>
           <t>33319-5764</t>
         </is>
@@ -1431,58 +1507,64 @@
         <v>11</v>
       </c>
       <c r="I13" t="n">
+        <v>11</v>
+      </c>
+      <c r="J13" t="n">
+        <v>11</v>
+      </c>
+      <c r="K13" t="n">
         <v>116877515</v>
       </c>
-      <c r="J13" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K13" t="inlineStr">
+      <c r="L13" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M13" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>COSO-20-002324</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>Johanna</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr">
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr">
         <is>
           <t>Nunez</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr">
+      <c r="T13" t="inlineStr">
         <is>
           <t>11201 SW 55 STREET #307</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="U13" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="T13" t="inlineStr">
+      <c r="V13" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U13" t="n">
+      <c r="W13" t="n">
         <v>33025</v>
       </c>
     </row>
@@ -1512,58 +1594,64 @@
         <v>12</v>
       </c>
       <c r="I14" t="n">
+        <v>12</v>
+      </c>
+      <c r="J14" t="n">
+        <v>12</v>
+      </c>
+      <c r="K14" t="n">
         <v>116877519</v>
       </c>
-      <c r="J14" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K14" t="inlineStr">
+      <c r="L14" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M14" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>COCE-20-024861</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>Gabriel</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr">
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr">
         <is>
           <t>Vermenton</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
+      <c r="T14" t="inlineStr">
         <is>
           <t>5078 S UNIVERSITY DRIVE</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="U14" t="inlineStr">
         <is>
           <t>DAVIE</t>
         </is>
       </c>
-      <c r="T14" t="inlineStr">
+      <c r="V14" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U14" t="inlineStr">
+      <c r="W14" t="inlineStr">
         <is>
           <t>33328-4509</t>
         </is>
@@ -1595,58 +1683,64 @@
         <v>13</v>
       </c>
       <c r="I15" t="n">
+        <v>13</v>
+      </c>
+      <c r="J15" t="n">
+        <v>13</v>
+      </c>
+      <c r="K15" t="n">
         <v>116877641</v>
       </c>
-      <c r="J15" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K15" t="inlineStr">
+      <c r="L15" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M15" t="inlineStr">
         <is>
           <t>Cavalry Spv I LLC</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>COCE-20-001654</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>Valycia</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr">
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr">
         <is>
           <t>Cureton</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr">
+      <c r="T15" t="inlineStr">
         <is>
           <t>10140 NW 4 COURT</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="U15" t="inlineStr">
         <is>
           <t>PEMBROKE PINES</t>
         </is>
       </c>
-      <c r="T15" t="inlineStr">
+      <c r="V15" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U15" t="inlineStr">
+      <c r="W15" t="inlineStr">
         <is>
           <t>33026-3977</t>
         </is>
@@ -1678,58 +1772,64 @@
         <v>14</v>
       </c>
       <c r="I16" t="n">
+        <v>14</v>
+      </c>
+      <c r="J16" t="n">
+        <v>14</v>
+      </c>
+      <c r="K16" t="n">
         <v>116877648</v>
       </c>
-      <c r="J16" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>COCE-20-008634</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>Ayed</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr">
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr">
         <is>
           <t>Mohammed</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>4125 NW 65 AVENUE</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
+      <c r="U16" t="inlineStr">
         <is>
           <t>CORAL SPRINGS</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr">
+      <c r="V16" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U16" t="inlineStr">
+      <c r="W16" t="inlineStr">
         <is>
           <t>33067-3037</t>
         </is>
@@ -1761,62 +1861,68 @@
         <v>15</v>
       </c>
       <c r="I17" t="n">
+        <v>15</v>
+      </c>
+      <c r="J17" t="n">
+        <v>15</v>
+      </c>
+      <c r="K17" t="n">
         <v>116877675</v>
       </c>
-      <c r="J17" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K17" t="inlineStr">
+      <c r="L17" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M17" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
+      <c r="P17" t="inlineStr">
         <is>
           <t>COCE-20-008636</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
+      <c r="Q17" t="inlineStr">
         <is>
           <t>Marica</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
+      <c r="R17" t="inlineStr">
         <is>
           <t>Christie</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
+      <c r="S17" t="inlineStr">
         <is>
           <t>Hamilton</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr">
+      <c r="T17" t="inlineStr">
         <is>
           <t>6058 SW 19 STREET</t>
         </is>
       </c>
-      <c r="S17" t="inlineStr">
+      <c r="U17" t="inlineStr">
         <is>
           <t>NORTH LAUDERDALE</t>
         </is>
       </c>
-      <c r="T17" t="inlineStr">
+      <c r="V17" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U17" t="inlineStr">
+      <c r="W17" t="inlineStr">
         <is>
           <t>33068-4613</t>
         </is>
@@ -1848,42 +1954,48 @@
         <v>16</v>
       </c>
       <c r="I18" t="n">
+        <v>16</v>
+      </c>
+      <c r="J18" t="n">
+        <v>16</v>
+      </c>
+      <c r="K18" t="n">
         <v>116877677</v>
       </c>
-      <c r="J18" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K18" t="inlineStr">
+      <c r="L18" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M18" t="inlineStr">
         <is>
           <t>Petersburg Hospital Company LLC</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr">
+        <is>
           <t>CONO-17-002495</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="Q18" t="inlineStr">
         <is>
           <t>Leila</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr">
         <is>
           <t>Mazzone</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1911,58 +2023,64 @@
         <v>17</v>
       </c>
       <c r="I19" t="n">
+        <v>17</v>
+      </c>
+      <c r="J19" t="n">
+        <v>17</v>
+      </c>
+      <c r="K19" t="n">
         <v>116877679</v>
       </c>
-      <c r="J19" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K19" t="inlineStr">
+      <c r="L19" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M19" t="inlineStr">
         <is>
           <t>Cavalry Spv I LLC</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
+      <c r="P19" t="inlineStr">
         <is>
           <t>COCE-20-008435</t>
         </is>
       </c>
-      <c r="O19" t="inlineStr">
+      <c r="Q19" t="inlineStr">
         <is>
           <t>Murry</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr">
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr">
         <is>
           <t>Schlessinger</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr">
+      <c r="T19" t="inlineStr">
         <is>
           <t>2521 NW 104 AVE #207</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
+      <c r="U19" t="inlineStr">
         <is>
           <t>SUNRISE</t>
         </is>
       </c>
-      <c r="T19" t="inlineStr">
+      <c r="V19" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U19" t="inlineStr">
+      <c r="W19" t="inlineStr">
         <is>
           <t>33322-6348</t>
         </is>
@@ -1994,58 +2112,64 @@
         <v>18</v>
       </c>
       <c r="I20" t="n">
+        <v>18</v>
+      </c>
+      <c r="J20" t="n">
+        <v>18</v>
+      </c>
+      <c r="K20" t="n">
         <v>116877684</v>
       </c>
-      <c r="J20" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K20" t="inlineStr">
+      <c r="L20" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M20" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
+      <c r="P20" t="inlineStr">
         <is>
           <t>COCE-20-008403</t>
         </is>
       </c>
-      <c r="O20" t="inlineStr">
+      <c r="Q20" t="inlineStr">
         <is>
           <t>Keith</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr">
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr">
         <is>
           <t>Salomon</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr">
+      <c r="T20" t="inlineStr">
         <is>
           <t>6550 SW 27 PLACE</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
+      <c r="U20" t="inlineStr">
         <is>
           <t>MIRAMAR</t>
         </is>
       </c>
-      <c r="T20" t="inlineStr">
+      <c r="V20" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U20" t="inlineStr">
+      <c r="W20" t="inlineStr">
         <is>
           <t>33023-3838</t>
         </is>
@@ -2077,46 +2201,52 @@
         <v>19</v>
       </c>
       <c r="I21" t="n">
+        <v>19</v>
+      </c>
+      <c r="J21" t="n">
+        <v>19</v>
+      </c>
+      <c r="K21" t="n">
         <v>116877690</v>
       </c>
-      <c r="J21" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K21" t="inlineStr">
+      <c r="L21" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M21" t="inlineStr">
         <is>
           <t>Cavalry Spv I LLC</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr">
+        <is>
           <t>COWE-17-004647</t>
         </is>
       </c>
-      <c r="O21" t="inlineStr">
+      <c r="Q21" t="inlineStr">
         <is>
           <t>Franklin</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr">
+      <c r="R21" t="inlineStr">
         <is>
           <t>J</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
+      <c r="S21" t="inlineStr">
         <is>
           <t>Barahona</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2144,62 +2274,68 @@
         <v>20</v>
       </c>
       <c r="I22" t="n">
+        <v>20</v>
+      </c>
+      <c r="J22" t="n">
+        <v>20</v>
+      </c>
+      <c r="K22" t="n">
         <v>116877691</v>
       </c>
-      <c r="J22" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K22" t="inlineStr">
+      <c r="L22" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M22" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N22" t="inlineStr">
+      <c r="P22" t="inlineStr">
         <is>
           <t>COCE-20-008605</t>
         </is>
       </c>
-      <c r="O22" t="inlineStr">
+      <c r="Q22" t="inlineStr">
         <is>
           <t>Ayanna</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr">
+      <c r="R22" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
+      <c r="S22" t="inlineStr">
         <is>
           <t>Streete</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr">
+      <c r="T22" t="inlineStr">
         <is>
           <t>7715 YARDLEY DRIVE #109</t>
         </is>
       </c>
-      <c r="S22" t="inlineStr">
+      <c r="U22" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="T22" t="inlineStr">
+      <c r="V22" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U22" t="inlineStr">
+      <c r="W22" t="inlineStr">
         <is>
           <t>33321-0859</t>
         </is>
@@ -2231,58 +2367,64 @@
         <v>21</v>
       </c>
       <c r="I23" t="n">
+        <v>21</v>
+      </c>
+      <c r="J23" t="n">
+        <v>21</v>
+      </c>
+      <c r="K23" t="n">
         <v>116877693</v>
       </c>
-      <c r="J23" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K23" t="inlineStr">
+      <c r="L23" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M23" t="inlineStr">
         <is>
           <t>Midland Credit Management Inc</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N23" t="inlineStr">
+      <c r="P23" t="inlineStr">
         <is>
           <t>COCE-20-020540</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr">
+      <c r="Q23" t="inlineStr">
         <is>
           <t>Robert</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr">
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr">
         <is>
           <t>Knapp</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr">
+      <c r="T23" t="inlineStr">
         <is>
           <t>1570 NW 128 DRIVE #110</t>
         </is>
       </c>
-      <c r="S23" t="inlineStr">
+      <c r="U23" t="inlineStr">
         <is>
           <t>SUNRISE</t>
         </is>
       </c>
-      <c r="T23" t="inlineStr">
+      <c r="V23" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U23" t="inlineStr">
+      <c r="W23" t="inlineStr">
         <is>
           <t>33323-5215</t>
         </is>
@@ -2314,58 +2456,64 @@
         <v>22</v>
       </c>
       <c r="I24" t="n">
+        <v>22</v>
+      </c>
+      <c r="J24" t="n">
+        <v>22</v>
+      </c>
+      <c r="K24" t="n">
         <v>116877708</v>
       </c>
-      <c r="J24" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K24" t="inlineStr">
+      <c r="L24" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M24" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N24" t="inlineStr">
+      <c r="P24" t="inlineStr">
         <is>
           <t>COCE-20-024840</t>
         </is>
       </c>
-      <c r="O24" t="inlineStr">
+      <c r="Q24" t="inlineStr">
         <is>
           <t>Jonathan</t>
         </is>
       </c>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr">
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr">
         <is>
           <t>Duque</t>
         </is>
       </c>
-      <c r="R24" t="inlineStr">
+      <c r="T24" t="inlineStr">
         <is>
           <t>17404 SW 31 COURT</t>
         </is>
       </c>
-      <c r="S24" t="inlineStr">
+      <c r="U24" t="inlineStr">
         <is>
           <t>MIRAMAR</t>
         </is>
       </c>
-      <c r="T24" t="inlineStr">
+      <c r="V24" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U24" t="inlineStr">
+      <c r="W24" t="inlineStr">
         <is>
           <t>33029-5588</t>
         </is>
@@ -2397,58 +2545,64 @@
         <v>23</v>
       </c>
       <c r="I25" t="n">
+        <v>23</v>
+      </c>
+      <c r="J25" t="n">
+        <v>23</v>
+      </c>
+      <c r="K25" t="n">
         <v>116877709</v>
       </c>
-      <c r="J25" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K25" t="inlineStr">
+      <c r="L25" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M25" t="inlineStr">
         <is>
           <t>Cavalry Spv I LLC</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N25" t="inlineStr">
+      <c r="P25" t="inlineStr">
         <is>
           <t>COCE-20-001491</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="Q25" t="inlineStr">
         <is>
           <t>Rachel</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr">
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr">
         <is>
           <t>Lacroix</t>
         </is>
       </c>
-      <c r="R25" t="inlineStr">
+      <c r="T25" t="inlineStr">
         <is>
           <t>8837 ANDORA DRIVE</t>
         </is>
       </c>
-      <c r="S25" t="inlineStr">
+      <c r="U25" t="inlineStr">
         <is>
           <t>MIRAMAR</t>
         </is>
       </c>
-      <c r="T25" t="inlineStr">
+      <c r="V25" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U25" t="inlineStr">
+      <c r="W25" t="inlineStr">
         <is>
           <t>33025-2558</t>
         </is>
@@ -2480,58 +2634,64 @@
         <v>24</v>
       </c>
       <c r="I26" t="n">
+        <v>24</v>
+      </c>
+      <c r="J26" t="n">
+        <v>24</v>
+      </c>
+      <c r="K26" t="n">
         <v>116877721</v>
       </c>
-      <c r="J26" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K26" t="inlineStr">
+      <c r="L26" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M26" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N26" t="inlineStr">
+      <c r="P26" t="inlineStr">
         <is>
           <t>COSO-18-007361</t>
         </is>
       </c>
-      <c r="O26" t="inlineStr">
+      <c r="Q26" t="inlineStr">
         <is>
           <t>Joseph</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr">
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr">
         <is>
           <t>Jean</t>
         </is>
       </c>
-      <c r="R26" t="inlineStr">
+      <c r="T26" t="inlineStr">
         <is>
           <t>15819 NW 11 STREET</t>
         </is>
       </c>
-      <c r="S26" t="inlineStr">
+      <c r="U26" t="inlineStr">
         <is>
           <t>PEMBROKE PINES</t>
         </is>
       </c>
-      <c r="T26" t="inlineStr">
+      <c r="V26" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U26" t="n">
+      <c r="W26" t="n">
         <v>33028</v>
       </c>
     </row>
@@ -2561,58 +2721,64 @@
         <v>25</v>
       </c>
       <c r="I27" t="n">
+        <v>25</v>
+      </c>
+      <c r="J27" t="n">
+        <v>25</v>
+      </c>
+      <c r="K27" t="n">
         <v>116877726</v>
       </c>
-      <c r="J27" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K27" t="inlineStr">
+      <c r="L27" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M27" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N27" t="inlineStr">
+      <c r="P27" t="inlineStr">
         <is>
           <t>COCE-20-024782</t>
         </is>
       </c>
-      <c r="O27" t="inlineStr">
+      <c r="Q27" t="inlineStr">
         <is>
           <t>Nicole</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr">
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr">
         <is>
           <t>Kuhar</t>
         </is>
       </c>
-      <c r="R27" t="inlineStr">
+      <c r="T27" t="inlineStr">
         <is>
           <t>4840 NE 5 AVENUE</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr">
+      <c r="U27" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="T27" t="inlineStr">
+      <c r="V27" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U27" t="inlineStr">
+      <c r="W27" t="inlineStr">
         <is>
           <t>33334-2322</t>
         </is>
@@ -2644,62 +2810,68 @@
         <v>26</v>
       </c>
       <c r="I28" t="n">
+        <v>26</v>
+      </c>
+      <c r="J28" t="n">
+        <v>26</v>
+      </c>
+      <c r="K28" t="n">
         <v>116877737</v>
       </c>
-      <c r="J28" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K28" t="inlineStr">
+      <c r="L28" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M28" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N28" t="inlineStr">
+      <c r="P28" t="inlineStr">
         <is>
           <t>COCE-20-008401</t>
         </is>
       </c>
-      <c r="O28" t="inlineStr">
+      <c r="Q28" t="inlineStr">
         <is>
           <t>Noah</t>
         </is>
       </c>
-      <c r="P28" t="inlineStr">
+      <c r="R28" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="Q28" t="inlineStr">
+      <c r="S28" t="inlineStr">
         <is>
           <t>Jones</t>
         </is>
       </c>
-      <c r="R28" t="inlineStr">
+      <c r="T28" t="inlineStr">
         <is>
           <t>7466 NW 47 PLACE</t>
         </is>
       </c>
-      <c r="S28" t="inlineStr">
+      <c r="U28" t="inlineStr">
         <is>
           <t>LAUDERHILL</t>
         </is>
       </c>
-      <c r="T28" t="inlineStr">
+      <c r="V28" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U28" t="inlineStr">
+      <c r="W28" t="inlineStr">
         <is>
           <t>33319-3416</t>
         </is>
@@ -2731,58 +2903,64 @@
         <v>27</v>
       </c>
       <c r="I29" t="n">
+        <v>27</v>
+      </c>
+      <c r="J29" t="n">
+        <v>27</v>
+      </c>
+      <c r="K29" t="n">
         <v>116877742</v>
       </c>
-      <c r="J29" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K29" t="inlineStr">
+      <c r="L29" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M29" t="inlineStr">
         <is>
           <t>Capital One Bank Usa</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N29" t="inlineStr">
+      <c r="P29" t="inlineStr">
         <is>
           <t>COCE-18-027671</t>
         </is>
       </c>
-      <c r="O29" t="inlineStr">
+      <c r="Q29" t="inlineStr">
         <is>
           <t>Stefanie</t>
         </is>
       </c>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr">
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr">
         <is>
           <t>Rodriguez</t>
         </is>
       </c>
-      <c r="R29" t="inlineStr">
+      <c r="T29" t="inlineStr">
         <is>
           <t>1141 NE 17 AVENUE #3</t>
         </is>
       </c>
-      <c r="S29" t="inlineStr">
+      <c r="U29" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="T29" t="inlineStr">
+      <c r="V29" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U29" t="n">
+      <c r="W29" t="n">
         <v>33304</v>
       </c>
     </row>
@@ -2812,62 +2990,68 @@
         <v>28</v>
       </c>
       <c r="I30" t="n">
+        <v>28</v>
+      </c>
+      <c r="J30" t="n">
+        <v>28</v>
+      </c>
+      <c r="K30" t="n">
         <v>116877760</v>
       </c>
-      <c r="J30" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K30" t="inlineStr">
+      <c r="L30" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M30" t="inlineStr">
         <is>
           <t>Wynmoor Nassau Village Assn Inc</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="N30" t="inlineStr">
+      <c r="P30" t="inlineStr">
         <is>
           <t>CONO-20-013473</t>
         </is>
       </c>
-      <c r="O30" t="inlineStr">
+      <c r="Q30" t="inlineStr">
         <is>
           <t>Richard</t>
         </is>
       </c>
-      <c r="P30" t="inlineStr">
+      <c r="R30" t="inlineStr">
         <is>
           <t>Jr</t>
         </is>
       </c>
-      <c r="Q30" t="inlineStr">
+      <c r="S30" t="inlineStr">
         <is>
           <t>Udovich</t>
         </is>
       </c>
-      <c r="R30" t="inlineStr">
+      <c r="T30" t="inlineStr">
         <is>
           <t>2710 NASSAU BEND #F1</t>
         </is>
       </c>
-      <c r="S30" t="inlineStr">
+      <c r="U30" t="inlineStr">
         <is>
           <t>COCONUT CREEK</t>
         </is>
       </c>
-      <c r="T30" t="inlineStr">
+      <c r="V30" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U30" t="n">
+      <c r="W30" t="n">
         <v>33066</v>
       </c>
     </row>
@@ -2897,58 +3081,64 @@
         <v>29</v>
       </c>
       <c r="I31" t="n">
+        <v>29</v>
+      </c>
+      <c r="J31" t="n">
+        <v>29</v>
+      </c>
+      <c r="K31" t="n">
         <v>116877785</v>
       </c>
-      <c r="J31" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K31" t="inlineStr">
+      <c r="L31" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M31" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N31" t="inlineStr">
+      <c r="P31" t="inlineStr">
         <is>
           <t>COCE-20-009469</t>
         </is>
       </c>
-      <c r="O31" t="inlineStr">
+      <c r="Q31" t="inlineStr">
         <is>
           <t>Michelle</t>
         </is>
       </c>
-      <c r="P31" t="inlineStr"/>
-      <c r="Q31" t="inlineStr">
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr">
         <is>
           <t>Hughes</t>
         </is>
       </c>
-      <c r="R31" t="inlineStr">
+      <c r="T31" t="inlineStr">
         <is>
           <t>2544 NW 99 AVENUE</t>
         </is>
       </c>
-      <c r="S31" t="inlineStr">
+      <c r="U31" t="inlineStr">
         <is>
           <t>CORAL SPRINGS</t>
         </is>
       </c>
-      <c r="T31" t="inlineStr">
+      <c r="V31" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U31" t="inlineStr">
+      <c r="W31" t="inlineStr">
         <is>
           <t>33065-6207</t>
         </is>
@@ -2980,58 +3170,64 @@
         <v>30</v>
       </c>
       <c r="I32" t="n">
+        <v>30</v>
+      </c>
+      <c r="J32" t="n">
+        <v>30</v>
+      </c>
+      <c r="K32" t="n">
         <v>116877826</v>
       </c>
-      <c r="J32" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K32" t="inlineStr">
+      <c r="L32" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M32" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N32" t="inlineStr">
+      <c r="P32" t="inlineStr">
         <is>
           <t>COCE-20-015574</t>
         </is>
       </c>
-      <c r="O32" t="inlineStr">
+      <c r="Q32" t="inlineStr">
         <is>
           <t>Jackie</t>
         </is>
       </c>
-      <c r="P32" t="inlineStr"/>
-      <c r="Q32" t="inlineStr">
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr">
         <is>
           <t>Alexander</t>
         </is>
       </c>
-      <c r="R32" t="inlineStr">
+      <c r="T32" t="inlineStr">
         <is>
           <t>1626 S 17 AVENUE</t>
         </is>
       </c>
-      <c r="S32" t="inlineStr">
+      <c r="U32" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="T32" t="inlineStr">
+      <c r="V32" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U32" t="inlineStr">
+      <c r="W32" t="inlineStr">
         <is>
           <t>33020-6535</t>
         </is>
@@ -3063,58 +3259,64 @@
         <v>31</v>
       </c>
       <c r="I33" t="n">
+        <v>31</v>
+      </c>
+      <c r="J33" t="n">
+        <v>31</v>
+      </c>
+      <c r="K33" t="n">
         <v>116877840</v>
       </c>
-      <c r="J33" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K33" t="inlineStr">
+      <c r="L33" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M33" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr">
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N33" t="inlineStr">
+      <c r="P33" t="inlineStr">
         <is>
           <t>COCE-20-015582</t>
         </is>
       </c>
-      <c r="O33" t="inlineStr">
+      <c r="Q33" t="inlineStr">
         <is>
           <t>Jennifer</t>
         </is>
       </c>
-      <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr">
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr">
         <is>
           <t>Matos</t>
         </is>
       </c>
-      <c r="R33" t="inlineStr">
+      <c r="T33" t="inlineStr">
         <is>
           <t>3777 NW 78 AVENUE #11F</t>
         </is>
       </c>
-      <c r="S33" t="inlineStr">
+      <c r="U33" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="T33" t="inlineStr">
+      <c r="V33" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U33" t="inlineStr">
+      <c r="W33" t="inlineStr">
         <is>
           <t>33024-8342</t>
         </is>
@@ -3146,58 +3348,64 @@
         <v>32</v>
       </c>
       <c r="I34" t="n">
+        <v>32</v>
+      </c>
+      <c r="J34" t="n">
+        <v>32</v>
+      </c>
+      <c r="K34" t="n">
         <v>116877868</v>
       </c>
-      <c r="J34" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K34" t="inlineStr">
+      <c r="L34" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M34" t="inlineStr">
         <is>
           <t>Tidewater Finance Company</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N34" t="inlineStr">
+      <c r="P34" t="inlineStr">
         <is>
           <t>COCE-20-023825</t>
         </is>
       </c>
-      <c r="O34" t="inlineStr">
+      <c r="Q34" t="inlineStr">
         <is>
           <t>Louisne</t>
         </is>
       </c>
-      <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr">
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr">
         <is>
           <t>Joseph</t>
         </is>
       </c>
-      <c r="R34" t="inlineStr">
+      <c r="T34" t="inlineStr">
         <is>
           <t>6391 SW 34 STREET</t>
         </is>
       </c>
-      <c r="S34" t="inlineStr">
+      <c r="U34" t="inlineStr">
         <is>
           <t>MIRAMAR</t>
         </is>
       </c>
-      <c r="T34" t="inlineStr">
+      <c r="V34" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U34" t="n">
+      <c r="W34" t="n">
         <v>33023</v>
       </c>
     </row>
@@ -3227,58 +3435,64 @@
         <v>33</v>
       </c>
       <c r="I35" t="n">
+        <v>33</v>
+      </c>
+      <c r="J35" t="n">
+        <v>33</v>
+      </c>
+      <c r="K35" t="n">
         <v>116877871</v>
       </c>
-      <c r="J35" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K35" t="inlineStr">
+      <c r="L35" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M35" t="inlineStr">
         <is>
           <t>Platinum Public Adjusters Inc</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="N35" t="inlineStr">
+      <c r="P35" t="inlineStr">
         <is>
           <t>COCE-20-009956</t>
         </is>
       </c>
-      <c r="O35" t="inlineStr">
+      <c r="Q35" t="inlineStr">
         <is>
           <t>Alvin</t>
         </is>
       </c>
-      <c r="P35" t="inlineStr"/>
-      <c r="Q35" t="inlineStr">
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr">
         <is>
           <t>Gray</t>
         </is>
       </c>
-      <c r="R35" t="inlineStr">
+      <c r="T35" t="inlineStr">
         <is>
           <t>3174 NW 43 STREET</t>
         </is>
       </c>
-      <c r="S35" t="inlineStr">
+      <c r="U35" t="inlineStr">
         <is>
           <t>FT LAUDERDALE</t>
         </is>
       </c>
-      <c r="T35" t="inlineStr">
+      <c r="V35" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U35" t="n">
+      <c r="W35" t="n">
         <v>33309</v>
       </c>
     </row>
@@ -3308,58 +3522,64 @@
         <v>34</v>
       </c>
       <c r="I36" t="n">
+        <v>34</v>
+      </c>
+      <c r="J36" t="n">
+        <v>34</v>
+      </c>
+      <c r="K36" t="n">
         <v>116877906</v>
       </c>
-      <c r="J36" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K36" t="inlineStr">
+      <c r="L36" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M36" t="inlineStr">
         <is>
           <t>Unifund Ccr LLC</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N36" t="inlineStr">
+      <c r="P36" t="inlineStr">
         <is>
           <t>COCE-20-015657</t>
         </is>
       </c>
-      <c r="O36" t="inlineStr">
+      <c r="Q36" t="inlineStr">
         <is>
           <t>Julia</t>
         </is>
       </c>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr">
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr">
         <is>
           <t>Mizaur</t>
         </is>
       </c>
-      <c r="R36" t="inlineStr">
+      <c r="T36" t="inlineStr">
         <is>
           <t>2336 TAFT STREET</t>
         </is>
       </c>
-      <c r="S36" t="inlineStr">
+      <c r="U36" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="T36" t="inlineStr">
+      <c r="V36" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U36" t="n">
+      <c r="W36" t="n">
         <v>33020</v>
       </c>
     </row>
@@ -3389,58 +3609,64 @@
         <v>35</v>
       </c>
       <c r="I37" t="n">
+        <v>35</v>
+      </c>
+      <c r="J37" t="n">
+        <v>35</v>
+      </c>
+      <c r="K37" t="n">
         <v>116877910</v>
       </c>
-      <c r="J37" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K37" t="inlineStr">
+      <c r="L37" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M37" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N37" t="inlineStr">
+      <c r="P37" t="inlineStr">
         <is>
           <t>COCE-20-008433</t>
         </is>
       </c>
-      <c r="O37" t="inlineStr">
+      <c r="Q37" t="inlineStr">
         <is>
           <t>Carmen</t>
         </is>
       </c>
-      <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr">
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr">
         <is>
           <t>Mora</t>
         </is>
       </c>
-      <c r="R37" t="inlineStr">
+      <c r="T37" t="inlineStr">
         <is>
           <t>3917 E SHORE ROAD</t>
         </is>
       </c>
-      <c r="S37" t="inlineStr">
+      <c r="U37" t="inlineStr">
         <is>
           <t>MIRAMAR</t>
         </is>
       </c>
-      <c r="T37" t="inlineStr">
+      <c r="V37" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U37" t="inlineStr">
+      <c r="W37" t="inlineStr">
         <is>
           <t>33023-4959</t>
         </is>
@@ -3472,58 +3698,64 @@
         <v>36</v>
       </c>
       <c r="I38" t="n">
+        <v>36</v>
+      </c>
+      <c r="J38" t="n">
+        <v>36</v>
+      </c>
+      <c r="K38" t="n">
         <v>116877929</v>
       </c>
-      <c r="J38" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K38" t="inlineStr">
+      <c r="L38" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M38" t="inlineStr">
         <is>
           <t>Portfolio Recovery Associates LLC</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N38" t="inlineStr">
+      <c r="P38" t="inlineStr">
         <is>
           <t>COCE-20-008434</t>
         </is>
       </c>
-      <c r="O38" t="inlineStr">
+      <c r="Q38" t="inlineStr">
         <is>
           <t>Andres</t>
         </is>
       </c>
-      <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr">
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr">
         <is>
           <t>Sanchez</t>
         </is>
       </c>
-      <c r="R38" t="inlineStr">
+      <c r="T38" t="inlineStr">
         <is>
           <t>1425 SAINT GABRIELLE LANE</t>
         </is>
       </c>
-      <c r="S38" t="inlineStr">
+      <c r="U38" t="inlineStr">
         <is>
           <t>WESTON</t>
         </is>
       </c>
-      <c r="T38" t="inlineStr">
+      <c r="V38" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U38" t="inlineStr">
+      <c r="W38" t="inlineStr">
         <is>
           <t>33326-4029</t>
         </is>
@@ -3555,42 +3787,48 @@
         <v>37</v>
       </c>
       <c r="I39" t="n">
+        <v>37</v>
+      </c>
+      <c r="J39" t="n">
+        <v>37</v>
+      </c>
+      <c r="K39" t="n">
         <v>116878464</v>
       </c>
-      <c r="J39" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K39" t="inlineStr">
+      <c r="L39" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M39" t="inlineStr">
         <is>
           <t>Cach LLC</t>
         </is>
       </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr">
         <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr">
+        <is>
           <t>CONO-13-009293</t>
         </is>
       </c>
-      <c r="O39" t="inlineStr">
+      <c r="Q39" t="inlineStr">
         <is>
           <t>Marie</t>
         </is>
       </c>
-      <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr">
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr">
         <is>
           <t>Stphard</t>
         </is>
       </c>
-      <c r="R39" t="inlineStr"/>
-      <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -3618,42 +3856,48 @@
         <v>38</v>
       </c>
       <c r="I40" t="n">
+        <v>38</v>
+      </c>
+      <c r="J40" t="n">
+        <v>38</v>
+      </c>
+      <c r="K40" t="n">
         <v>116878760</v>
       </c>
-      <c r="J40" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K40" t="inlineStr">
+      <c r="L40" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M40" t="inlineStr">
         <is>
           <t>Arrow Financial Services LLC</t>
         </is>
       </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr">
         <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr">
+        <is>
           <t>COWE-10-018019</t>
         </is>
       </c>
-      <c r="O40" t="inlineStr">
+      <c r="Q40" t="inlineStr">
         <is>
           <t>Corence</t>
         </is>
       </c>
-      <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr">
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr">
         <is>
           <t>Chisholm</t>
         </is>
       </c>
-      <c r="R40" t="inlineStr"/>
-      <c r="S40" t="inlineStr"/>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -3681,46 +3925,52 @@
         <v>39</v>
       </c>
       <c r="I41" t="n">
+        <v>39</v>
+      </c>
+      <c r="J41" t="n">
+        <v>39</v>
+      </c>
+      <c r="K41" t="n">
         <v>116878793</v>
       </c>
-      <c r="J41" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K41" t="inlineStr">
+      <c r="L41" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M41" t="inlineStr">
         <is>
           <t>Progressive Select Ins Co</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr">
         <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr">
+        <is>
           <t>COWE-20-010184</t>
         </is>
       </c>
-      <c r="O41" t="inlineStr">
+      <c r="Q41" t="inlineStr">
         <is>
           <t>Dakota</t>
         </is>
       </c>
-      <c r="P41" t="inlineStr">
+      <c r="R41" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="Q41" t="inlineStr">
+      <c r="S41" t="inlineStr">
         <is>
           <t>Mcquiston</t>
         </is>
       </c>
-      <c r="R41" t="inlineStr"/>
-      <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -3748,46 +3998,52 @@
         <v>40</v>
       </c>
       <c r="I42" t="n">
+        <v>40</v>
+      </c>
+      <c r="J42" t="n">
+        <v>40</v>
+      </c>
+      <c r="K42" t="n">
         <v>116878798</v>
       </c>
-      <c r="J42" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K42" t="inlineStr">
+      <c r="L42" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M42" t="inlineStr">
         <is>
           <t>Progressive Select Ins Co</t>
         </is>
       </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr">
         <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr">
+        <is>
           <t>COWE-20-010052</t>
         </is>
       </c>
-      <c r="O42" t="inlineStr">
+      <c r="Q42" t="inlineStr">
         <is>
           <t>Jarvierre</t>
         </is>
       </c>
-      <c r="P42" t="inlineStr">
+      <c r="R42" t="inlineStr">
         <is>
           <t>Deontaye</t>
         </is>
       </c>
-      <c r="Q42" t="inlineStr">
+      <c r="S42" t="inlineStr">
         <is>
           <t>Rogers</t>
         </is>
       </c>
-      <c r="R42" t="inlineStr"/>
-      <c r="S42" t="inlineStr"/>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -3815,62 +4071,68 @@
         <v>41</v>
       </c>
       <c r="I43" t="n">
+        <v>41</v>
+      </c>
+      <c r="J43" t="n">
+        <v>41</v>
+      </c>
+      <c r="K43" t="n">
         <v>116878808</v>
       </c>
-      <c r="J43" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K43" t="inlineStr">
+      <c r="L43" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M43" t="inlineStr">
         <is>
           <t>Progressive Select Insurance Company</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N43" t="inlineStr">
+      <c r="P43" t="inlineStr">
         <is>
           <t>COWE-20-020167</t>
         </is>
       </c>
-      <c r="O43" t="inlineStr">
+      <c r="Q43" t="inlineStr">
         <is>
           <t>Julio</t>
         </is>
       </c>
-      <c r="P43" t="inlineStr">
+      <c r="R43" t="inlineStr">
         <is>
           <t>R</t>
         </is>
       </c>
-      <c r="Q43" t="inlineStr">
+      <c r="S43" t="inlineStr">
         <is>
           <t>Rojas</t>
         </is>
       </c>
-      <c r="R43" t="inlineStr">
+      <c r="T43" t="inlineStr">
         <is>
           <t>7440 SW 36 STREET</t>
         </is>
       </c>
-      <c r="S43" t="inlineStr">
+      <c r="U43" t="inlineStr">
         <is>
           <t>DAVIE</t>
         </is>
       </c>
-      <c r="T43" t="inlineStr">
+      <c r="V43" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U43" t="n">
+      <c r="W43" t="n">
         <v>33314</v>
       </c>
     </row>
@@ -3900,58 +4162,64 @@
         <v>42</v>
       </c>
       <c r="I44" t="n">
+        <v>42</v>
+      </c>
+      <c r="J44" t="n">
+        <v>42</v>
+      </c>
+      <c r="K44" t="n">
         <v>116879076</v>
       </c>
-      <c r="J44" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K44" t="inlineStr">
+      <c r="L44" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M44" t="inlineStr">
         <is>
           <t>Dept Stores National Bank</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N44" t="inlineStr">
+      <c r="P44" t="inlineStr">
         <is>
           <t>COWE-20-005199</t>
         </is>
       </c>
-      <c r="O44" t="inlineStr">
+      <c r="Q44" t="inlineStr">
         <is>
           <t>Anee</t>
         </is>
       </c>
-      <c r="P44" t="inlineStr"/>
-      <c r="Q44" t="inlineStr">
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr">
         <is>
           <t>Villalba</t>
         </is>
       </c>
-      <c r="R44" t="inlineStr">
+      <c r="T44" t="inlineStr">
         <is>
           <t>121 NW 21 STREET</t>
         </is>
       </c>
-      <c r="S44" t="inlineStr">
+      <c r="U44" t="inlineStr">
         <is>
           <t>POMPANO BEACH</t>
         </is>
       </c>
-      <c r="T44" t="inlineStr">
+      <c r="V44" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U44" t="n">
+      <c r="W44" t="n">
         <v>33060</v>
       </c>
     </row>
@@ -3981,46 +4249,52 @@
         <v>43</v>
       </c>
       <c r="I45" t="n">
+        <v>43</v>
+      </c>
+      <c r="J45" t="n">
+        <v>43</v>
+      </c>
+      <c r="K45" t="n">
         <v>116879414</v>
       </c>
-      <c r="J45" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K45" t="inlineStr">
+      <c r="L45" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M45" t="inlineStr">
         <is>
           <t>Aig Enterprise Corp</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr">
         <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr">
+        <is>
           <t>CONO-20-019654</t>
         </is>
       </c>
-      <c r="O45" t="inlineStr">
+      <c r="Q45" t="inlineStr">
         <is>
           <t>Robertson</t>
         </is>
       </c>
-      <c r="P45" t="inlineStr">
+      <c r="R45" t="inlineStr">
         <is>
           <t>Marcus</t>
         </is>
       </c>
-      <c r="Q45" t="inlineStr">
+      <c r="S45" t="inlineStr">
         <is>
           <t>Dean</t>
         </is>
       </c>
-      <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -4048,58 +4322,64 @@
         <v>44</v>
       </c>
       <c r="I46" t="n">
+        <v>44</v>
+      </c>
+      <c r="J46" t="n">
+        <v>44</v>
+      </c>
+      <c r="K46" t="n">
         <v>116879713</v>
       </c>
-      <c r="J46" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K46" t="inlineStr">
+      <c r="L46" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M46" t="inlineStr">
         <is>
           <t>Cavalry Spv I LLC</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N46" t="inlineStr">
+      <c r="P46" t="inlineStr">
         <is>
           <t>COCE-18-014639</t>
         </is>
       </c>
-      <c r="O46" t="inlineStr">
+      <c r="Q46" t="inlineStr">
         <is>
           <t>Marie</t>
         </is>
       </c>
-      <c r="P46" t="inlineStr"/>
-      <c r="Q46" t="inlineStr">
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr">
         <is>
           <t>Chery</t>
         </is>
       </c>
-      <c r="R46" t="inlineStr">
+      <c r="T46" t="inlineStr">
         <is>
           <t>140 NE 27 STREET</t>
         </is>
       </c>
-      <c r="S46" t="inlineStr">
+      <c r="U46" t="inlineStr">
         <is>
           <t>POMPANO BEACH</t>
         </is>
       </c>
-      <c r="T46" t="inlineStr">
+      <c r="V46" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U46" t="inlineStr">
+      <c r="W46" t="inlineStr">
         <is>
           <t>33064-3628</t>
         </is>
@@ -4131,58 +4411,64 @@
         <v>45</v>
       </c>
       <c r="I47" t="n">
+        <v>45</v>
+      </c>
+      <c r="J47" t="n">
+        <v>45</v>
+      </c>
+      <c r="K47" t="n">
         <v>116879859</v>
       </c>
-      <c r="J47" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K47" t="inlineStr">
+      <c r="L47" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M47" t="inlineStr">
         <is>
           <t>Midland Credit Management Inc</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N47" t="inlineStr">
+      <c r="P47" t="inlineStr">
         <is>
           <t>COSO-20-002977</t>
         </is>
       </c>
-      <c r="O47" t="inlineStr">
+      <c r="Q47" t="inlineStr">
         <is>
           <t>Dianne</t>
         </is>
       </c>
-      <c r="P47" t="inlineStr"/>
-      <c r="Q47" t="inlineStr">
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr">
         <is>
           <t>Burgess</t>
         </is>
       </c>
-      <c r="R47" t="inlineStr">
+      <c r="T47" t="inlineStr">
         <is>
           <t>1080 S MILITARY TRAIL</t>
         </is>
       </c>
-      <c r="S47" t="inlineStr">
+      <c r="U47" t="inlineStr">
         <is>
           <t>DEERFIELD BEACH</t>
         </is>
       </c>
-      <c r="T47" t="inlineStr">
+      <c r="V47" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U47" t="inlineStr">
+      <c r="W47" t="inlineStr">
         <is>
           <t>33442-7691</t>
         </is>
@@ -4214,58 +4500,64 @@
         <v>46</v>
       </c>
       <c r="I48" t="n">
+        <v>46</v>
+      </c>
+      <c r="J48" t="n">
+        <v>46</v>
+      </c>
+      <c r="K48" t="n">
         <v>116879870</v>
       </c>
-      <c r="J48" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K48" t="inlineStr">
+      <c r="L48" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M48" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N48" t="inlineStr">
+      <c r="P48" t="inlineStr">
         <is>
           <t>COSO-19-015233</t>
         </is>
       </c>
-      <c r="O48" t="inlineStr">
+      <c r="Q48" t="inlineStr">
         <is>
           <t>Donald</t>
         </is>
       </c>
-      <c r="P48" t="inlineStr"/>
-      <c r="Q48" t="inlineStr">
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr">
         <is>
           <t>Siganoff</t>
         </is>
       </c>
-      <c r="R48" t="inlineStr">
+      <c r="T48" t="inlineStr">
         <is>
           <t>661 SE 2 TERRACE</t>
         </is>
       </c>
-      <c r="S48" t="inlineStr">
+      <c r="U48" t="inlineStr">
         <is>
           <t>POMPANO BEACH</t>
         </is>
       </c>
-      <c r="T48" t="inlineStr">
+      <c r="V48" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U48" t="n">
+      <c r="W48" t="n">
         <v>33060</v>
       </c>
     </row>
@@ -4295,58 +4587,64 @@
         <v>47</v>
       </c>
       <c r="I49" t="n">
+        <v>47</v>
+      </c>
+      <c r="J49" t="n">
+        <v>47</v>
+      </c>
+      <c r="K49" t="n">
         <v>116879890</v>
       </c>
-      <c r="J49" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K49" t="inlineStr">
+      <c r="L49" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M49" t="inlineStr">
         <is>
           <t>Midland Funding LLC</t>
         </is>
       </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="N49" t="inlineStr">
+      <c r="P49" t="inlineStr">
         <is>
           <t>COSO-19-010382</t>
         </is>
       </c>
-      <c r="O49" t="inlineStr">
+      <c r="Q49" t="inlineStr">
         <is>
           <t>Roberto</t>
         </is>
       </c>
-      <c r="P49" t="inlineStr"/>
-      <c r="Q49" t="inlineStr">
+      <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr">
         <is>
           <t>Martinez</t>
         </is>
       </c>
-      <c r="R49" t="inlineStr">
+      <c r="T49" t="inlineStr">
         <is>
           <t>2840 NE 7 TERRACE</t>
         </is>
       </c>
-      <c r="S49" t="inlineStr">
+      <c r="U49" t="inlineStr">
         <is>
           <t>POMPANO BEACH</t>
         </is>
       </c>
-      <c r="T49" t="inlineStr">
+      <c r="V49" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U49" t="n">
+      <c r="W49" t="n">
         <v>33064</v>
       </c>
     </row>
@@ -4376,62 +4674,68 @@
         <v>48</v>
       </c>
       <c r="I50" t="n">
+        <v>48</v>
+      </c>
+      <c r="J50" t="n">
+        <v>48</v>
+      </c>
+      <c r="K50" t="n">
         <v>116879960</v>
       </c>
-      <c r="J50" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K50" t="inlineStr">
+      <c r="L50" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M50" t="inlineStr">
         <is>
           <t>Jefferson Capital Systems LLC</t>
         </is>
       </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="N50" t="inlineStr">
+      <c r="P50" t="inlineStr">
         <is>
           <t>COSO-20-003012</t>
         </is>
       </c>
-      <c r="O50" t="inlineStr">
+      <c r="Q50" t="inlineStr">
         <is>
           <t>Jorge</t>
         </is>
       </c>
-      <c r="P50" t="inlineStr">
+      <c r="R50" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="Q50" t="inlineStr">
+      <c r="S50" t="inlineStr">
         <is>
           <t>Dieppa</t>
         </is>
       </c>
-      <c r="R50" t="inlineStr">
+      <c r="T50" t="inlineStr">
         <is>
           <t>7560 POLK STREET</t>
         </is>
       </c>
-      <c r="S50" t="inlineStr">
+      <c r="U50" t="inlineStr">
         <is>
           <t>HOLLYWOOD</t>
         </is>
       </c>
-      <c r="T50" t="inlineStr">
+      <c r="V50" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U50" t="n">
+      <c r="W50" t="n">
         <v>33024</v>
       </c>
     </row>
@@ -4461,58 +4765,64 @@
         <v>49</v>
       </c>
       <c r="I51" t="n">
+        <v>49</v>
+      </c>
+      <c r="J51" t="n">
+        <v>49</v>
+      </c>
+      <c r="K51" t="n">
         <v>116879961</v>
       </c>
-      <c r="J51" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K51" t="inlineStr">
+      <c r="L51" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M51" t="inlineStr">
         <is>
           <t>Velocity Investments LLC</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N51" t="inlineStr">
+      <c r="P51" t="inlineStr">
         <is>
           <t>COSO-20-009463</t>
         </is>
       </c>
-      <c r="O51" t="inlineStr">
+      <c r="Q51" t="inlineStr">
         <is>
           <t>Simon</t>
         </is>
       </c>
-      <c r="P51" t="inlineStr"/>
-      <c r="Q51" t="inlineStr">
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr">
         <is>
           <t>Hernandez</t>
         </is>
       </c>
-      <c r="R51" t="inlineStr">
+      <c r="T51" t="inlineStr">
         <is>
           <t>16711 SAPPHIRE ISLE</t>
         </is>
       </c>
-      <c r="S51" t="inlineStr">
+      <c r="U51" t="inlineStr">
         <is>
           <t>WESTON</t>
         </is>
       </c>
-      <c r="T51" t="inlineStr">
+      <c r="V51" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U51" t="n">
+      <c r="W51" t="n">
         <v>33331</v>
       </c>
     </row>
@@ -4542,58 +4852,64 @@
         <v>50</v>
       </c>
       <c r="I52" t="n">
+        <v>50</v>
+      </c>
+      <c r="J52" t="n">
+        <v>50</v>
+      </c>
+      <c r="K52" t="n">
         <v>116879962</v>
       </c>
-      <c r="J52" s="2" t="n">
-        <v>44155</v>
-      </c>
-      <c r="K52" t="inlineStr">
+      <c r="L52" s="2" t="n">
+        <v>44155</v>
+      </c>
+      <c r="M52" t="inlineStr">
         <is>
           <t>Velocity Investments LLC</t>
         </is>
       </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="N52" t="inlineStr">
+      <c r="P52" t="inlineStr">
         <is>
           <t>COSO-19-006341</t>
         </is>
       </c>
-      <c r="O52" t="inlineStr">
+      <c r="Q52" t="inlineStr">
         <is>
           <t>Patricia</t>
         </is>
       </c>
-      <c r="P52" t="inlineStr"/>
-      <c r="Q52" t="inlineStr">
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr">
         <is>
           <t>Garcia</t>
         </is>
       </c>
-      <c r="R52" t="inlineStr">
+      <c r="T52" t="inlineStr">
         <is>
           <t>581 SE 13 STREET #106</t>
         </is>
       </c>
-      <c r="S52" t="inlineStr">
+      <c r="U52" t="inlineStr">
         <is>
           <t>DANIA BEACH</t>
         </is>
       </c>
-      <c r="T52" t="inlineStr">
+      <c r="V52" t="inlineStr">
         <is>
           <t>FL</t>
         </is>
       </c>
-      <c r="U52" t="n">
+      <c r="W52" t="n">
         <v>33004</v>
       </c>
     </row>

</xml_diff>